<commit_message>
Now there is weather data and the gas demand is computed per month with load profiles
</commit_message>
<xml_diff>
--- a/Buildings/Residential/Required_energy_2014.xlsx
+++ b/Buildings/Residential/Required_energy_2014.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10133" uniqueCount="961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10201" uniqueCount="998">
   <si>
     <t xml:space="preserve">Code_BuildingVariant</t>
   </si>
@@ -2768,6 +2768,18 @@
     <t xml:space="preserve">AVG people</t>
   </si>
   <si>
+    <t xml:space="preserve">Gas demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of apartments afected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrogen needed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Required power</t>
   </si>
   <si>
@@ -2777,6 +2789,18 @@
     <t xml:space="preserve">number of 1000s buildings</t>
   </si>
   <si>
+    <t xml:space="preserve">kWh/yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ton CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tonH2/yr</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
@@ -2817,6 +2841,93 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.arcgis.com/home/item.html?id=b6a82e2a656042b899bb88a1aeca5751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total demand Mwh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mCO2/mCH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values for H2 retrofitted boilers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E/kgCH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh/kgCH4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH4 eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas demand Mwh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E/kgH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh/kgH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ph2/Ptot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 boiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas demand after criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% apartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twh/yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kgH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot apartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twh NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mton CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mton H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">601 Twh is in the right order of magnitude as can be seen here : https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/natural-gas/021623-german-gas-consumption-remains-in-critical-range-in-week-6-regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this article it is said that German consumption between 2018-21 was of 1,938 Twh/d for Households and small commercial businesses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This comes to 707.37 Twh/yr</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -2922,7 +3033,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
@@ -2931,11 +3042,14 @@
     <numFmt numFmtId="169" formatCode="General"/>
     <numFmt numFmtId="170" formatCode="0.00"/>
     <numFmt numFmtId="171" formatCode="0"/>
-    <numFmt numFmtId="172" formatCode="0.00\ %"/>
-    <numFmt numFmtId="173" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
-    <numFmt numFmtId="174" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="0.000E+00"/>
+    <numFmt numFmtId="173" formatCode="0.00\ %"/>
+    <numFmt numFmtId="174" formatCode="#,##0"/>
+    <numFmt numFmtId="175" formatCode="0.00000"/>
+    <numFmt numFmtId="176" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
+    <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2978,6 +3092,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2986,6 +3107,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -3052,7 +3174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -3088,6 +3210,20 @@
       <bottom style="thin">
         <color rgb="FFEAEAEA"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -3140,7 +3276,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3189,7 +3325,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3197,15 +3357,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3213,11 +3381,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3364,11 +3540,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -3474,17 +3655,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="64099474"/>
-        <c:axId val="61753940"/>
+        <c:axId val="24406194"/>
+        <c:axId val="58349270"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64099474"/>
+        <c:axId val="24406194"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3501,17 +3682,21 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61753940"/>
+        <c:crossAx val="58349270"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61753940"/>
+        <c:axId val="58349270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3526,7 +3711,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3543,14 +3728,18 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64099474"/>
+        <c:crossAx val="24406194"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3586,9 +3775,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>289800</xdr:colOff>
+      <xdr:colOff>288000</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>73800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3596,8 +3785,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7752240" y="1549440"/>
-        <a:ext cx="5753880" cy="3240360"/>
+        <a:off x="7758360" y="1549440"/>
+        <a:ext cx="5761080" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3727,7 +3916,7 @@
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="40.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.69"/>
@@ -68292,22 +68481,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB91"/>
+  <dimension ref="A1:BN91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="AL3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="AZ16" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="topRight" activeCell="AL1" activeCellId="0" sqref="AL1"/>
-      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
-      <selection pane="bottomRight" activeCell="AY13" activeCellId="0" sqref="AY13"/>
+      <selection pane="topRight" activeCell="AZ1" activeCellId="0" sqref="AZ1"/>
+      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="BI63" activeCellId="0" sqref="BI63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="47" style="1" width="13.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="47" style="1" width="13.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -68440,6 +68629,20 @@
       <c r="AU1" s="1" t="s">
         <v>910</v>
       </c>
+      <c r="AW1" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="BB1" s="1"/>
+      <c r="BC1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
@@ -68551,10 +68754,10 @@
         <v>74</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>911</v>
+        <v>915</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="AQ2" s="1" t="s">
         <v>76</v>
@@ -68563,12 +68766,30 @@
         <v>77</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>913</v>
+        <v>917</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>918</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>914</v>
-      </c>
-      <c r="AZ2" s="4" t="n">
+        <v>919</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="BJ2" s="4" t="n">
         <v>0.00330964757397794</v>
       </c>
     </row>
@@ -68628,10 +68849,14 @@
       <c r="AR3" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AY3" s="1" t="s">
-        <v>915</v>
-      </c>
-      <c r="AZ3" s="3" t="n">
+      <c r="BE3" s="1"/>
+      <c r="BF3" s="1"/>
+      <c r="BG3" s="1"/>
+      <c r="BH3" s="1"/>
+      <c r="BI3" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="BJ3" s="3" t="n">
         <v>1.03812774928714</v>
       </c>
     </row>
@@ -68707,16 +68932,16 @@
         <v>93</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>916</v>
+        <v>924</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>917</v>
+        <v>925</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="AW4" s="5" t="s">
-        <v>918</v>
+        <v>925</v>
+      </c>
+      <c r="AY4" s="5" t="s">
+        <v>926</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -68806,17 +69031,21 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
-      <c r="AW5" s="6" t="s">
-        <v>919</v>
-      </c>
-      <c r="AY5" s="1" t="s">
-        <v>920</v>
-      </c>
-      <c r="AZ5" s="1" t="n">
+      <c r="AY5" s="6" t="s">
+        <v>927</v>
+      </c>
+      <c r="BE5" s="1"/>
+      <c r="BF5" s="1"/>
+      <c r="BG5" s="1"/>
+      <c r="BH5" s="1"/>
+      <c r="BI5" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="BJ5" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="BA5" s="1" t="s">
-        <v>921</v>
+      <c r="BK5" s="1" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -68943,17 +69172,21 @@
       <c r="AS6" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AY6" s="1" t="s">
-        <v>922</v>
-      </c>
-      <c r="AZ6" s="1" t="n">
+      <c r="BE6" s="1"/>
+      <c r="BF6" s="1"/>
+      <c r="BG6" s="1"/>
+      <c r="BH6" s="1"/>
+      <c r="BI6" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="BJ6" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="BA6" s="1" t="s">
-        <v>917</v>
-      </c>
-      <c r="BB6" s="2" t="s">
-        <v>923</v>
+      <c r="BK6" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="BL6" s="2" t="s">
+        <v>931</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -69060,12 +69293,12 @@
         <v>294.244950471126</v>
       </c>
       <c r="AM7" s="7" t="n">
-        <f aca="false">AJ7*M7/X7/$AZ$5</f>
+        <f aca="false">AJ7*M7/X7/$BJ$5</f>
         <v>64.474694352482</v>
       </c>
       <c r="AN7" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM7^$AZ$3</f>
-        <v>1.25063042034891</v>
+        <f aca="false">$BJ$2*$BJ$8*AM7^$BJ$3</f>
+        <v>1.25063042034889</v>
       </c>
       <c r="AQ7" s="9" t="n">
         <v>1</v>
@@ -69077,16 +69310,31 @@
         <v>370</v>
       </c>
       <c r="AT7" s="10" t="n">
-        <f aca="false">$AZ$6*AQ7*$AZ$11</f>
+        <f aca="false">$BJ$6*AQ7*$BJ$11</f>
         <v>0.6</v>
       </c>
       <c r="AU7" s="11" t="n">
-        <f aca="false">SUMPRODUCT(AZ11*AQ7:AQ17 , AS7:AS17) / SUM(AS7:AS17)</f>
+        <f aca="false">SUMPRODUCT(BJ11*AQ7:AQ17 , AS7:AS17) / SUM(AS7:AS17)</f>
         <v>2.24806201550388</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>924</v>
-      </c>
+        <v>932</v>
+      </c>
+      <c r="AW7" s="1" t="n">
+        <f aca="false">AJ7*M7*AS7*1000/$BJ$17</f>
+        <v>4778781085.52394</v>
+      </c>
+      <c r="AY7" s="1" t="n">
+        <f aca="false">(AW7/$BJ$14)*$BJ$13/1000</f>
+        <v>819238.340109021</v>
+      </c>
+      <c r="AZ7" s="12" t="n">
+        <f aca="false">AS7*AQ7*1000</f>
+        <v>370000</v>
+      </c>
+      <c r="BA7" s="12"/>
+      <c r="BB7" s="12"/>
+      <c r="BC7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -69192,11 +69440,11 @@
         <v>280.580877709067</v>
       </c>
       <c r="AM8" s="7" t="n">
-        <f aca="false">AJ8*M8/X8/$AZ$5</f>
+        <f aca="false">AJ8*M8/X8/$BJ$5</f>
         <v>39.823386036405</v>
       </c>
       <c r="AN8" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM8^$AZ$3</f>
+        <f aca="false">$BJ$2*$BJ$8*AM8^$BJ$3</f>
         <v>0.758402238479523</v>
       </c>
       <c r="AQ8" s="9" t="n">
@@ -69209,18 +69457,40 @@
         <v>1040</v>
       </c>
       <c r="AT8" s="10" t="n">
-        <f aca="false">$AZ$6*AQ8</f>
+        <f aca="false">$BJ$6*AQ8</f>
         <v>0.3</v>
       </c>
       <c r="AU8" s="1" t="n">
         <f aca="false">MEDIAN(AQ7:AQ19)</f>
         <v>1</v>
       </c>
-      <c r="AY8" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="AZ8" s="1" t="n">
+      <c r="AW8" s="1" t="n">
+        <f aca="false">AJ8*M8*AS8*1000/$BJ$17</f>
+        <v>8296552066.64996</v>
+      </c>
+      <c r="AY8" s="1" t="n">
+        <f aca="false">(AW8/$BJ$14)*$BJ$13/1000</f>
+        <v>1422298.57825035</v>
+      </c>
+      <c r="AZ8" s="12" t="n">
+        <f aca="false">AS8*AQ8*1000</f>
+        <v>1040000</v>
+      </c>
+      <c r="BA8" s="12"/>
+      <c r="BB8" s="12"/>
+      <c r="BC8" s="12"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="BJ8" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="BK8" s="1" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69327,12 +69597,12 @@
         <v>227.424386756216</v>
       </c>
       <c r="AM9" s="7" t="n">
-        <f aca="false">AJ9*M9/X9/$AZ$5</f>
+        <f aca="false">AJ9*M9/X9/$BJ$5</f>
         <v>68.8647417354908</v>
       </c>
       <c r="AN9" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM9^$AZ$3</f>
-        <v>1.33914425935902</v>
+        <f aca="false">$BJ$2*$BJ$8*AM9^$BJ$3</f>
+        <v>1.339144259359</v>
       </c>
       <c r="AQ9" s="9" t="n">
         <v>2</v>
@@ -69344,9 +69614,24 @@
         <v>1280</v>
       </c>
       <c r="AT9" s="10" t="n">
-        <f aca="false">$AZ$6*AQ9</f>
+        <f aca="false">$BJ$6*AQ9</f>
         <v>0.6</v>
       </c>
+      <c r="AW9" s="1" t="n">
+        <f aca="false">AJ9*M9*AS9*1000/$BJ$17</f>
+        <v>17657654411.8722</v>
+      </c>
+      <c r="AY9" s="1" t="n">
+        <f aca="false">(AW9/$BJ$14)*$BJ$13/1000</f>
+        <v>3027095.66136464</v>
+      </c>
+      <c r="AZ9" s="12" t="n">
+        <f aca="false">AS9*AQ9*1000</f>
+        <v>2560000</v>
+      </c>
+      <c r="BA9" s="12"/>
+      <c r="BB9" s="12"/>
+      <c r="BC9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -69452,12 +69737,12 @@
         <v>284.077290407009</v>
       </c>
       <c r="AM10" s="7" t="n">
-        <f aca="false">AJ10*M10/X10/$AZ$5</f>
+        <f aca="false">AJ10*M10/X10/$BJ$5</f>
         <v>31.5925795437625</v>
       </c>
       <c r="AN10" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM10^$AZ$3</f>
-        <v>0.596365686014433</v>
+        <f aca="false">$BJ$2*$BJ$8*AM10^$BJ$3</f>
+        <v>0.596365686014426</v>
       </c>
       <c r="AQ10" s="9" t="n">
         <v>1</v>
@@ -69469,9 +69754,24 @@
         <v>920</v>
       </c>
       <c r="AT10" s="10" t="n">
-        <f aca="false">$AZ$6*AQ10</f>
+        <f aca="false">$BJ$6*AQ10</f>
         <v>0.3</v>
       </c>
+      <c r="AW10" s="1" t="n">
+        <f aca="false">AJ10*M10*AS10*1000/$BJ$17</f>
+        <v>5822359736.73174</v>
+      </c>
+      <c r="AY10" s="1" t="n">
+        <f aca="false">(AW10/$BJ$14)*$BJ$13/1000</f>
+        <v>998141.626676908</v>
+      </c>
+      <c r="AZ10" s="12" t="n">
+        <f aca="false">AS10*AQ10*1000</f>
+        <v>920000</v>
+      </c>
+      <c r="BA10" s="12"/>
+      <c r="BB10" s="12"/>
+      <c r="BC10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -69577,12 +69877,12 @@
         <v>275.634619575176</v>
       </c>
       <c r="AM11" s="7" t="n">
-        <f aca="false">AJ11*M11/X11/$AZ$5</f>
+        <f aca="false">AJ11*M11/X11/$BJ$5</f>
         <v>33.4458744593622</v>
       </c>
       <c r="AN11" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM11^$AZ$3</f>
-        <v>0.632723640041757</v>
+        <f aca="false">$BJ$2*$BJ$8*AM11^$BJ$3</f>
+        <v>0.632723640041749</v>
       </c>
       <c r="AQ11" s="9" t="n">
         <v>1</v>
@@ -69594,17 +69894,34 @@
         <v>1580</v>
       </c>
       <c r="AT11" s="10" t="n">
-        <f aca="false">$AZ$6*AQ11</f>
+        <f aca="false">$BJ$6*AQ11</f>
         <v>0.3</v>
       </c>
-      <c r="AY11" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="AZ11" s="1" t="n">
+      <c r="AW11" s="1" t="n">
+        <f aca="false">AJ11*M11*AS11*1000/$BJ$17</f>
+        <v>10585850644.505</v>
+      </c>
+      <c r="AY11" s="1" t="n">
+        <f aca="false">(AW11/$BJ$14)*$BJ$13/1000</f>
+        <v>1814758.73354334</v>
+      </c>
+      <c r="AZ11" s="12" t="n">
+        <f aca="false">AS11*AQ11*1000</f>
+        <v>1580000</v>
+      </c>
+      <c r="BA11" s="12"/>
+      <c r="BB11" s="12"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="BJ11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="BA11" s="1" t="s">
-        <v>927</v>
+      <c r="BK11" s="1" t="s">
+        <v>935</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69711,12 +70028,12 @@
         <v>203.273144350112</v>
       </c>
       <c r="AM12" s="7" t="n">
-        <f aca="false">AJ12*M12/X12/$AZ$5</f>
+        <f aca="false">AJ12*M12/X12/$BJ$5</f>
         <v>35.2523245832401</v>
       </c>
       <c r="AN12" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM12^$AZ$3</f>
-        <v>0.668236666904083</v>
+        <f aca="false">$BJ$2*$BJ$8*AM12^$BJ$3</f>
+        <v>0.668236666904075</v>
       </c>
       <c r="AQ12" s="9" t="n">
         <v>1</v>
@@ -69728,9 +70045,24 @@
         <v>1470</v>
       </c>
       <c r="AT12" s="10" t="n">
-        <f aca="false">$AZ$6*AQ12</f>
+        <f aca="false">$BJ$6*AQ12</f>
         <v>0.3</v>
       </c>
+      <c r="AW12" s="1" t="n">
+        <f aca="false">AJ12*M12*AS12*1000/$BJ$17</f>
+        <v>10380809348.3508</v>
+      </c>
+      <c r="AY12" s="1" t="n">
+        <f aca="false">(AW12/$BJ$14)*$BJ$13/1000</f>
+        <v>1779607.99361428</v>
+      </c>
+      <c r="AZ12" s="12" t="n">
+        <f aca="false">AS12*AQ12*1000</f>
+        <v>1470000</v>
+      </c>
+      <c r="BA12" s="12"/>
+      <c r="BB12" s="12"/>
+      <c r="BC12" s="12"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -69836,12 +70168,12 @@
         <v>135.762996176219</v>
       </c>
       <c r="AM13" s="7" t="n">
-        <f aca="false">AJ13*M13/X13/$AZ$5</f>
+        <f aca="false">AJ13*M13/X13/$BJ$5</f>
         <v>29.2998017773702</v>
       </c>
       <c r="AN13" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM13^$AZ$3</f>
-        <v>0.551498945050836</v>
+        <f aca="false">$BJ$2*$BJ$8*AM13^$BJ$3</f>
+        <v>0.55149894505083</v>
       </c>
       <c r="AQ13" s="9" t="n">
         <v>1</v>
@@ -69853,8 +70185,35 @@
         <v>750</v>
       </c>
       <c r="AT13" s="10" t="n">
-        <f aca="false">$AZ$6*AQ13</f>
+        <f aca="false">$BJ$6*AQ13</f>
         <v>0.3</v>
+      </c>
+      <c r="AW13" s="1" t="n">
+        <f aca="false">AJ13*M13*AS13*1000/$BJ$17</f>
+        <v>4402020549.76832</v>
+      </c>
+      <c r="AY13" s="1" t="n">
+        <f aca="false">(AW13/$BJ$14)*$BJ$13/1000</f>
+        <v>754649.343373846</v>
+      </c>
+      <c r="AZ13" s="12" t="n">
+        <f aca="false">AS13*AQ13*1000</f>
+        <v>750000</v>
+      </c>
+      <c r="BA13" s="12"/>
+      <c r="BB13" s="12"/>
+      <c r="BC13" s="12"/>
+      <c r="BE13" s="1"/>
+      <c r="BF13" s="1"/>
+      <c r="BG13" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="BH13" s="1"/>
+      <c r="BI13" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="BJ13" s="1" t="n">
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69961,12 +70320,12 @@
         <v>157.912973629207</v>
       </c>
       <c r="AM14" s="7" t="n">
-        <f aca="false">AJ14*M14/X14/$AZ$5</f>
+        <f aca="false">AJ14*M14/X14/$BJ$5</f>
         <v>23.7430612652403</v>
       </c>
       <c r="AN14" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM14^$AZ$3</f>
-        <v>0.443337621572041</v>
+        <f aca="false">$BJ$2*$BJ$8*AM14^$BJ$3</f>
+        <v>0.443337621572036</v>
       </c>
       <c r="AQ14" s="9" t="n">
         <v>1</v>
@@ -69978,8 +70337,48 @@
         <v>1040</v>
       </c>
       <c r="AT14" s="10" t="n">
-        <f aca="false">$AZ$6*AQ14</f>
+        <f aca="false">$BJ$6*AQ14</f>
         <v>0.3</v>
+      </c>
+      <c r="AW14" s="1" t="n">
+        <f aca="false">AJ14*M14*AS14*1000/$BJ$17</f>
+        <v>4946479031.90977</v>
+      </c>
+      <c r="AY14" s="1" t="n">
+        <f aca="false">(AW14/$BJ$14)*$BJ$13/1000</f>
+        <v>847987.216606627</v>
+      </c>
+      <c r="AZ14" s="12" t="n">
+        <f aca="false">AS14*AQ14*1000</f>
+        <v>1040000</v>
+      </c>
+      <c r="BA14" s="12"/>
+      <c r="BB14" s="12"/>
+      <c r="BC14" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="BD14" s="13"/>
+      <c r="BE14" s="13"/>
+      <c r="BF14" s="1"/>
+      <c r="BG14" s="14" t="n">
+        <f aca="false">SUM(AW7:AW16)/1000</f>
+        <v>71983839.4872346</v>
+      </c>
+      <c r="BH14" s="1"/>
+      <c r="BI14" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="BJ14" s="1" t="n">
+        <v>14.583</v>
+      </c>
+      <c r="BK14" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="BM14" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="BN14" s="15" t="n">
+        <v>0.94</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70086,12 +70485,12 @@
         <v>122.597588442444</v>
       </c>
       <c r="AM15" s="7" t="n">
-        <f aca="false">AJ15*M15/X15/$AZ$5</f>
+        <f aca="false">AJ15*M15/X15/$BJ$5</f>
         <v>14.9571512305957</v>
       </c>
       <c r="AN15" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM15^$AZ$3</f>
-        <v>0.274406872148005</v>
+        <f aca="false">$BJ$2*$BJ$8*AM15^$BJ$3</f>
+        <v>0.274406872148002</v>
       </c>
       <c r="AQ15" s="9" t="n">
         <v>1</v>
@@ -70103,8 +70502,43 @@
         <v>1080</v>
       </c>
       <c r="AT15" s="10" t="n">
-        <f aca="false">$AZ$6*AQ15</f>
+        <f aca="false">$BJ$6*AQ15</f>
         <v>0.3</v>
+      </c>
+      <c r="AW15" s="1" t="n">
+        <f aca="false">AJ15*M15*AS15*1000/$BJ$17</f>
+        <v>3235927332.20659</v>
+      </c>
+      <c r="AY15" s="1" t="n">
+        <f aca="false">(AW15/$BJ$14)*$BJ$13/1000</f>
+        <v>554743.079648665</v>
+      </c>
+      <c r="BA15" s="1" t="n">
+        <f aca="false">(AW15/$BJ$15/$BN$15)/1000</f>
+        <v>116972.926167554</v>
+      </c>
+      <c r="BB15" s="1"/>
+      <c r="BC15" s="1"/>
+      <c r="BE15" s="1"/>
+      <c r="BF15" s="1"/>
+      <c r="BG15" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="BJ15" s="1" t="n">
+        <v>33.33</v>
+      </c>
+      <c r="BK15" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="BM15" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="BN15" s="15" t="n">
+        <v>0.83</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70211,12 +70645,12 @@
         <v>80.8860079579963</v>
       </c>
       <c r="AM16" s="7" t="n">
-        <f aca="false">AJ16*M16/X16/$AZ$5</f>
+        <f aca="false">AJ16*M16/X16/$BJ$5</f>
         <v>11.8632811671728</v>
       </c>
       <c r="AN16" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM16^$AZ$3</f>
-        <v>0.215731513690938</v>
+        <f aca="false">$BJ$2*$BJ$8*AM16^$BJ$3</f>
+        <v>0.215731513690936</v>
       </c>
       <c r="AQ16" s="9" t="n">
         <v>1</v>
@@ -70228,8 +70662,35 @@
         <v>790</v>
       </c>
       <c r="AT16" s="10" t="n">
-        <f aca="false">$AZ$6*AQ16</f>
+        <f aca="false">$BJ$6*AQ16</f>
         <v>0.3</v>
+      </c>
+      <c r="AW16" s="1" t="n">
+        <f aca="false">AJ16*M16*AS16*1000/$BJ$17</f>
+        <v>1877405279.71615</v>
+      </c>
+      <c r="AY16" s="1" t="n">
+        <f aca="false">(AW16/$BJ$14)*$BJ$13/1000</f>
+        <v>321848.261625891</v>
+      </c>
+      <c r="BA16" s="1" t="n">
+        <f aca="false">(AW16/$BJ$15/$BN$15)/1000</f>
+        <v>67864.808639279</v>
+      </c>
+      <c r="BB16" s="1"/>
+      <c r="BC16" s="12" t="s">
+        <v>946</v>
+      </c>
+      <c r="BD16" s="8" t="n">
+        <f aca="false">(AW15+AW16)/SUM(AW7:AW16)</f>
+        <v>0.0710344522929974</v>
+      </c>
+      <c r="BE16" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BG16" s="16" t="n">
+        <f aca="false">BD16*SUM(AW7:AW16)/1000</f>
+        <v>5113332.61192274</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -70342,12 +70803,12 @@
         <v>82.1959469992663</v>
       </c>
       <c r="AM17" s="7" t="n">
-        <f aca="false">AJ17*M17/X17/$AZ$5</f>
+        <f aca="false">AJ17*M17/X17/$BJ$5</f>
         <v>15.7965050405997</v>
       </c>
       <c r="AN17" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM17^$AZ$3</f>
-        <v>0.290409754096317</v>
+        <f aca="false">$BJ$2*$BJ$8*AM17^$BJ$3</f>
+        <v>0.290409754096314</v>
       </c>
       <c r="AQ17" s="9" t="n">
         <v>1</v>
@@ -70359,8 +70820,27 @@
         <v>0</v>
       </c>
       <c r="AT17" s="10" t="n">
-        <f aca="false">$AZ$6*AQ17</f>
+        <f aca="false">$BJ$6*AQ17</f>
         <v>0.3</v>
+      </c>
+      <c r="AW17" s="1" t="n">
+        <f aca="false">AJ17*M17*AS17*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="1"/>
+      <c r="BC17" s="1"/>
+      <c r="BI17" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="BJ17" s="1" t="n">
+        <v>4.987</v>
+      </c>
+      <c r="BK17" s="1" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -70473,12 +70953,12 @@
         <v>69.4841973336749</v>
       </c>
       <c r="AM18" s="7" t="n">
-        <f aca="false">AJ18*M18/X18/$AZ$5</f>
+        <f aca="false">AJ18*M18/X18/$BJ$5</f>
         <v>13.3535473888174</v>
       </c>
       <c r="AN18" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM18^$AZ$3</f>
-        <v>0.243929807962904</v>
+        <f aca="false">$BJ$2*$BJ$8*AM18^$BJ$3</f>
+        <v>0.243929807962902</v>
       </c>
       <c r="AQ18" s="9" t="n">
         <v>1</v>
@@ -70486,11 +70966,33 @@
       <c r="AR18" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="AS18" s="12"/>
+      <c r="AS18" s="17"/>
       <c r="AT18" s="10" t="n">
-        <f aca="false">$AZ$6*AQ18</f>
+        <f aca="false">$BJ$6*AQ18</f>
         <v>0.3</v>
       </c>
+      <c r="AW18" s="1" t="n">
+        <f aca="false">AJ18*M18*AS18*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="1"/>
+      <c r="BC18" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD18" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="BE18" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="BF18" s="1"/>
+      <c r="BG18" s="1"/>
+      <c r="BH18" s="1"/>
+      <c r="BI18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
@@ -70598,12 +71100,12 @@
         <v>132.14078844121</v>
       </c>
       <c r="AM19" s="7" t="n">
-        <f aca="false">AJ19*M19/X19/$AZ$5</f>
+        <f aca="false">AJ19*M19/X19/$BJ$5</f>
         <v>24.4440617657013</v>
       </c>
       <c r="AN19" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM19^$AZ$3</f>
-        <v>0.456933557086769</v>
+        <f aca="false">$BJ$2*$BJ$8*AM19^$BJ$3</f>
+        <v>0.456933557086764</v>
       </c>
       <c r="AQ19" s="9" t="n">
         <v>1</v>
@@ -70611,11 +71113,36 @@
       <c r="AR19" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AS19" s="12"/>
+      <c r="AS19" s="17"/>
       <c r="AT19" s="10" t="n">
-        <f aca="false">$AZ$6*AQ19</f>
+        <f aca="false">$BJ$6*AQ19</f>
         <v>0.3</v>
       </c>
+      <c r="AW19" s="1" t="n">
+        <f aca="false">AJ19*M19*AS19*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="1"/>
+      <c r="BB19" s="1"/>
+      <c r="BC19" s="1" t="n">
+        <f aca="false">SUM(AY7:AY14)</f>
+        <v>11463777.493539</v>
+      </c>
+      <c r="BD19" s="18" t="n">
+        <f aca="false">SUM(AZ7:AZ14)</f>
+        <v>9730000</v>
+      </c>
+      <c r="BE19" s="1" t="n">
+        <f aca="false">BA15+BA16</f>
+        <v>184837.734806833</v>
+      </c>
+      <c r="BF19" s="18"/>
+      <c r="BG19" s="18"/>
+      <c r="BH19" s="18"/>
+      <c r="BI19" s="18"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
@@ -70656,12 +71183,18 @@
       <c r="AJ20" s="2"/>
       <c r="AM20" s="7"/>
       <c r="AN20" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM20^$AZ$3</f>
+        <f aca="false">$BJ$2*$BJ$8*AM20^$BJ$3</f>
         <v>0</v>
       </c>
       <c r="AQ20" s="9"/>
       <c r="AR20" s="9"/>
       <c r="AT20" s="10"/>
+      <c r="AW20" s="1" t="n">
+        <f aca="false">AJ20*M20*AS20*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -70769,12 +71302,12 @@
         <v>207.433293099569</v>
       </c>
       <c r="AM21" s="7" t="n">
-        <f aca="false">AJ21*M21/X21/$AZ$5</f>
+        <f aca="false">AJ21*M21/X21/$BJ$5</f>
         <v>19.9260545936006</v>
       </c>
       <c r="AN21" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM21^$AZ$3</f>
-        <v>0.369587335474826</v>
+        <f aca="false">$BJ$2*$BJ$8*AM21^$BJ$3</f>
+        <v>0.369587335474822</v>
       </c>
       <c r="AQ21" s="9" t="n">
         <v>1</v>
@@ -70786,16 +71319,33 @@
         <v>350</v>
       </c>
       <c r="AT21" s="10" t="n">
-        <f aca="false">$AZ$6*AQ21</f>
+        <f aca="false">$BJ$6*AQ21</f>
         <v>0.3</v>
       </c>
       <c r="AU21" s="7" t="n">
-        <f aca="false">SUMPRODUCT(AZ11*AQ21:AQ29, AS21:AS29) / SUM(AS21:AS29)</f>
+        <f aca="false">SUMPRODUCT(BJ11*AQ21:AQ29, AS21:AS29) / SUM(AS21:AS29)</f>
         <v>2</v>
       </c>
       <c r="AV21" s="1" t="s">
-        <v>924</v>
-      </c>
+        <v>932</v>
+      </c>
+      <c r="AW21" s="1" t="n">
+        <f aca="false">AJ21*M21*AS21*1000/$BJ$17</f>
+        <v>1397061357.25937</v>
+      </c>
+      <c r="AY21" s="1" t="n">
+        <f aca="false">(AW21/$BJ$14)*$BJ$13/1000</f>
+        <v>239501.706997766</v>
+      </c>
+      <c r="AZ21" s="1" t="n">
+        <f aca="false">AS21*AQ21*1000</f>
+        <v>350000</v>
+      </c>
+      <c r="BA21" s="1" t="n">
+        <f aca="false">(AW21/$BJ$15/$BN$15)/1000</f>
+        <v>50501.2437602569</v>
+      </c>
+      <c r="BB21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -70903,12 +71453,12 @@
         <v>162.397385679511</v>
       </c>
       <c r="AM22" s="7" t="n">
-        <f aca="false">AJ22*M22/X22/$AZ$5</f>
+        <f aca="false">AJ22*M22/X22/$BJ$5</f>
         <v>18.3286338692341</v>
       </c>
       <c r="AN22" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM22^$AZ$3</f>
-        <v>0.338877050505106</v>
+        <f aca="false">$BJ$2*$BJ$8*AM22^$BJ$3</f>
+        <v>0.338877050505103</v>
       </c>
       <c r="AQ22" s="9" t="n">
         <v>1</v>
@@ -70920,13 +71470,30 @@
         <v>800</v>
       </c>
       <c r="AT22" s="10" t="n">
-        <f aca="false">$AZ$6*AQ22</f>
+        <f aca="false">$BJ$6*AQ22</f>
         <v>0.3</v>
       </c>
       <c r="AU22" s="1" t="n">
         <f aca="false">MEDIAN(AQ21:AQ31)</f>
         <v>1</v>
       </c>
+      <c r="AW22" s="1" t="n">
+        <f aca="false">AJ22*M22*AS22*1000/$BJ$17</f>
+        <v>2937285780.68817</v>
+      </c>
+      <c r="AY22" s="1" t="n">
+        <f aca="false">(AW22/$BJ$14)*$BJ$13/1000</f>
+        <v>503546.214888598</v>
+      </c>
+      <c r="AZ22" s="1" t="n">
+        <f aca="false">AS22*AQ22*1000</f>
+        <v>800000</v>
+      </c>
+      <c r="BA22" s="1" t="n">
+        <f aca="false">(AW22/$BJ$15/$BN$15)/1000</f>
+        <v>106177.573685857</v>
+      </c>
+      <c r="BB22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -71034,12 +71601,12 @@
         <v>201.20926055009</v>
       </c>
       <c r="AM23" s="7" t="n">
-        <f aca="false">AJ23*M23/X23/$AZ$5</f>
+        <f aca="false">AJ23*M23/X23/$BJ$5</f>
         <v>30.1310364147082</v>
       </c>
       <c r="AN23" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM23^$AZ$3</f>
-        <v>0.56775020924064</v>
+        <f aca="false">$BJ$2*$BJ$8*AM23^$BJ$3</f>
+        <v>0.567750209240634</v>
       </c>
       <c r="AQ23" s="9" t="n">
         <v>1</v>
@@ -71051,9 +71618,26 @@
         <v>480</v>
       </c>
       <c r="AT23" s="10" t="n">
-        <f aca="false">$AZ$6*AQ23</f>
+        <f aca="false">$BJ$6*AQ23</f>
         <v>0.3</v>
       </c>
+      <c r="AW23" s="1" t="n">
+        <f aca="false">AJ23*M23*AS23*1000/$BJ$17</f>
+        <v>2897219687.50368</v>
+      </c>
+      <c r="AY23" s="1" t="n">
+        <f aca="false">(AW23/$BJ$14)*$BJ$13/1000</f>
+        <v>496677.584773997</v>
+      </c>
+      <c r="AZ23" s="1" t="n">
+        <f aca="false">AS23*AQ23*1000</f>
+        <v>480000</v>
+      </c>
+      <c r="BA23" s="1" t="n">
+        <f aca="false">(AW23/$BJ$15/$BN$15)/1000</f>
+        <v>104729.256811356</v>
+      </c>
+      <c r="BB23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -71161,12 +71745,12 @@
         <v>111.374813767735</v>
       </c>
       <c r="AM24" s="7" t="n">
-        <f aca="false">AJ24*M24/X24/$AZ$5</f>
+        <f aca="false">AJ24*M24/X24/$BJ$5</f>
         <v>13.085147038958</v>
       </c>
       <c r="AN24" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM24^$AZ$3</f>
-        <v>0.238841954751617</v>
+        <f aca="false">$BJ$2*$BJ$8*AM24^$BJ$3</f>
+        <v>0.238841954751615</v>
       </c>
       <c r="AQ24" s="9" t="n">
         <v>1</v>
@@ -71178,9 +71762,22 @@
         <v>670</v>
       </c>
       <c r="AT24" s="10" t="n">
-        <f aca="false">$AZ$6*AQ24</f>
+        <f aca="false">$BJ$6*AQ24</f>
         <v>0.3</v>
       </c>
+      <c r="AW24" s="1" t="n">
+        <f aca="false">AJ24*M24*AS24*1000/$BJ$17</f>
+        <v>1756222471.94421</v>
+      </c>
+      <c r="AY24" s="1" t="n">
+        <f aca="false">(AW24/$BJ$14)*$BJ$13/1000</f>
+        <v>301073.591158234</v>
+      </c>
+      <c r="BA24" s="1" t="n">
+        <f aca="false">(AW24/$BJ$15/$BN$15)/1000</f>
+        <v>63484.2690995923</v>
+      </c>
+      <c r="BB24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -71288,12 +71885,12 @@
         <v>142.433950182057</v>
       </c>
       <c r="AM25" s="7" t="n">
-        <f aca="false">AJ25*M25/X25/$AZ$5</f>
+        <f aca="false">AJ25*M25/X25/$BJ$5</f>
         <v>15.1567687636074</v>
       </c>
       <c r="AN25" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM25^$AZ$3</f>
-        <v>0.278209690618705</v>
+        <f aca="false">$BJ$2*$BJ$8*AM25^$BJ$3</f>
+        <v>0.278209690618702</v>
       </c>
       <c r="AQ25" s="9" t="n">
         <v>1</v>
@@ -71305,8 +71902,24 @@
         <v>650</v>
       </c>
       <c r="AT25" s="10" t="n">
-        <f aca="false">$AZ$6*AQ25</f>
+        <f aca="false">$BJ$6*AQ25</f>
         <v>0.3</v>
+      </c>
+      <c r="AW25" s="1" t="n">
+        <f aca="false">AJ25*M25*AS25*1000/$BJ$17</f>
+        <v>1973540765.31952</v>
+      </c>
+      <c r="AY25" s="1" t="n">
+        <f aca="false">(AW25/$BJ$14)*$BJ$13/1000</f>
+        <v>338329.007289228</v>
+      </c>
+      <c r="BA25" s="1" t="n">
+        <f aca="false">(AW25/$BJ$15/$BN$15)/1000</f>
+        <v>71339.9327397627</v>
+      </c>
+      <c r="BB25" s="1"/>
+      <c r="BG25" s="1" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -71415,12 +72028,12 @@
         <v>143.274338056453</v>
       </c>
       <c r="AM26" s="7" t="n">
-        <f aca="false">AJ26*M26/X26/$AZ$5</f>
+        <f aca="false">AJ26*M26/X26/$BJ$5</f>
         <v>15.5282706750614</v>
       </c>
       <c r="AN26" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM26^$AZ$3</f>
-        <v>0.285292063529798</v>
+        <f aca="false">$BJ$2*$BJ$8*AM26^$BJ$3</f>
+        <v>0.285292063529796</v>
       </c>
       <c r="AQ26" s="9" t="n">
         <v>1</v>
@@ -71432,8 +72045,30 @@
         <v>380</v>
       </c>
       <c r="AT26" s="10" t="n">
-        <f aca="false">$AZ$6*AQ26</f>
+        <f aca="false">$BJ$6*AQ26</f>
         <v>0.3</v>
+      </c>
+      <c r="AW26" s="1" t="n">
+        <f aca="false">AJ26*M26*AS26*1000/$BJ$17</f>
+        <v>1182041731.23457</v>
+      </c>
+      <c r="AY26" s="1" t="n">
+        <f aca="false">(AW26/$BJ$14)*$BJ$13/1000</f>
+        <v>202640.35713409</v>
+      </c>
+      <c r="BA26" s="1" t="n">
+        <f aca="false">(AW26/$BJ$15/$BN$15)/1000</f>
+        <v>42728.6727914202</v>
+      </c>
+      <c r="BB26" s="1"/>
+      <c r="BC26" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="BD26" s="13"/>
+      <c r="BE26" s="13"/>
+      <c r="BG26" s="14" t="n">
+        <f aca="false">SUM(AW21:AW29)/1000</f>
+        <v>15366599.6960373</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -71542,12 +72177,12 @@
         <v>98.828096112019</v>
       </c>
       <c r="AM27" s="7" t="n">
-        <f aca="false">AJ27*M27/X27/$AZ$5</f>
+        <f aca="false">AJ27*M27/X27/$BJ$5</f>
         <v>12.6230881520457</v>
       </c>
       <c r="AN27" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM27^$AZ$3</f>
-        <v>0.230092433094793</v>
+        <f aca="false">$BJ$2*$BJ$8*AM27^$BJ$3</f>
+        <v>0.230092433094791</v>
       </c>
       <c r="AQ27" s="9" t="n">
         <v>1</v>
@@ -71559,8 +72194,24 @@
         <v>540</v>
       </c>
       <c r="AT27" s="10" t="n">
-        <f aca="false">$AZ$6*AQ27</f>
+        <f aca="false">$BJ$6*AQ27</f>
         <v>0.3</v>
+      </c>
+      <c r="AW27" s="1" t="n">
+        <f aca="false">AJ27*M27*AS27*1000/$BJ$17</f>
+        <v>1365480476.13847</v>
+      </c>
+      <c r="AY27" s="1" t="n">
+        <f aca="false">(AW27/$BJ$14)*$BJ$13/1000</f>
+        <v>234087.717914433</v>
+      </c>
+      <c r="BA27" s="1" t="n">
+        <f aca="false">(AW27/$BJ$15/$BN$15)/1000</f>
+        <v>49359.651970202</v>
+      </c>
+      <c r="BB27" s="1"/>
+      <c r="BG27" s="1" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -71669,12 +72320,12 @@
         <v>81.015865323379</v>
       </c>
       <c r="AM28" s="7" t="n">
-        <f aca="false">AJ28*M28/X28/$AZ$5</f>
+        <f aca="false">AJ28*M28/X28/$BJ$5</f>
         <v>12.0696608969755</v>
       </c>
       <c r="AN28" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM28^$AZ$3</f>
-        <v>0.219628867359612</v>
+        <f aca="false">$BJ$2*$BJ$8*AM28^$BJ$3</f>
+        <v>0.21962886735961</v>
       </c>
       <c r="AQ28" s="9" t="n">
         <v>1</v>
@@ -71686,8 +72337,35 @@
         <v>500</v>
       </c>
       <c r="AT28" s="10" t="n">
-        <f aca="false">$AZ$6*AQ28</f>
+        <f aca="false">$BJ$6*AQ28</f>
         <v>0.3</v>
+      </c>
+      <c r="AW28" s="1" t="n">
+        <f aca="false">AJ28*M28*AS28*1000/$BJ$17</f>
+        <v>1208902269.50857</v>
+      </c>
+      <c r="AY28" s="1" t="n">
+        <f aca="false">(AW28/$BJ$14)*$BJ$13/1000</f>
+        <v>207245.126090066</v>
+      </c>
+      <c r="BA28" s="1" t="n">
+        <f aca="false">(AW28/$BJ$15/$BN$15)/1000</f>
+        <v>43699.6327165935</v>
+      </c>
+      <c r="BB28" s="1"/>
+      <c r="BC28" s="12" t="s">
+        <v>946</v>
+      </c>
+      <c r="BD28" s="8" t="n">
+        <f aca="false">SUM(AY24:AY29)/SUM(AY21:AY29)</f>
+        <v>0.529397071017861</v>
+      </c>
+      <c r="BE28" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BG28" s="16" t="n">
+        <f aca="false">BD28*SUM(AW21:AW29)/1000</f>
+        <v>8135032.8705861</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -71796,12 +72474,12 @@
         <v>71.002365329692</v>
       </c>
       <c r="AM29" s="7" t="n">
-        <f aca="false">AJ29*M29/X29/$AZ$5</f>
+        <f aca="false">AJ29*M29/X29/$BJ$5</f>
         <v>10.7967660833168</v>
       </c>
       <c r="AN29" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM29^$AZ$3</f>
-        <v>0.195633223105913</v>
+        <f aca="false">$BJ$2*$BJ$8*AM29^$BJ$3</f>
+        <v>0.195633223105911</v>
       </c>
       <c r="AQ29" s="9" t="n">
         <v>1</v>
@@ -71813,9 +72491,22 @@
         <v>300</v>
       </c>
       <c r="AT29" s="10" t="n">
-        <f aca="false">$AZ$6*AQ29</f>
+        <f aca="false">$BJ$6*AQ29</f>
         <v>0.3</v>
       </c>
+      <c r="AW29" s="1" t="n">
+        <f aca="false">AJ29*M29*AS29*1000/$BJ$17</f>
+        <v>648845156.440757</v>
+      </c>
+      <c r="AY29" s="1" t="n">
+        <f aca="false">(AW29/$BJ$14)*$BJ$13/1000</f>
+        <v>111233.140718775</v>
+      </c>
+      <c r="BA29" s="1" t="n">
+        <f aca="false">(AW29/$BJ$15/$BN$15)/1000</f>
+        <v>23454.5800281507</v>
+      </c>
+      <c r="BB29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -71927,12 +72618,12 @@
         <v>69.8463359691521</v>
       </c>
       <c r="AM30" s="7" t="n">
-        <f aca="false">AJ30*M30/X30/$AZ$5</f>
+        <f aca="false">AJ30*M30/X30/$BJ$5</f>
         <v>14.0698689123045</v>
       </c>
       <c r="AN30" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM30^$AZ$3</f>
-        <v>0.257527446304821</v>
+        <f aca="false">$BJ$2*$BJ$8*AM30^$BJ$3</f>
+        <v>0.257527446304818</v>
       </c>
       <c r="AQ30" s="9" t="n">
         <v>1</v>
@@ -71940,11 +72631,37 @@
       <c r="AR30" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="AS30" s="12"/>
+      <c r="AS30" s="17"/>
       <c r="AT30" s="10" t="n">
-        <f aca="false">$AZ$6*AQ30</f>
+        <f aca="false">$BJ$6*AQ30</f>
         <v>0.3</v>
       </c>
+      <c r="AW30" s="1" t="n">
+        <f aca="false">AJ30*M30*AS30*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY30" s="1" t="n">
+        <f aca="false">(AW30/$BJ$14)*$BJ$13/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BA30" s="1" t="n">
+        <f aca="false">(AW30/$BJ$15/$BN$15)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BB30" s="1"/>
+      <c r="BC30" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD30" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="BE30" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="BF30" s="1"/>
+      <c r="BG30" s="1"/>
+      <c r="BH30" s="1"/>
+      <c r="BI30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -72056,12 +72773,12 @@
         <v>58.6222892112966</v>
       </c>
       <c r="AM31" s="7" t="n">
-        <f aca="false">AJ31*M31/X31/$AZ$5</f>
+        <f aca="false">AJ31*M31/X31/$BJ$5</f>
         <v>11.8088932382427</v>
       </c>
       <c r="AN31" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM31^$AZ$3</f>
-        <v>0.214704859761355</v>
+        <f aca="false">$BJ$2*$BJ$8*AM31^$BJ$3</f>
+        <v>0.214704859761353</v>
       </c>
       <c r="AQ31" s="9" t="n">
         <v>1</v>
@@ -72069,11 +72786,40 @@
       <c r="AR31" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="AS31" s="12"/>
+      <c r="AS31" s="17"/>
       <c r="AT31" s="10" t="n">
-        <f aca="false">$AZ$6*AQ31</f>
+        <f aca="false">$BJ$6*AQ31</f>
         <v>0.3</v>
       </c>
+      <c r="AW31" s="1" t="n">
+        <f aca="false">AJ31*M31*AS31*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY31" s="1" t="n">
+        <f aca="false">(AW31/$BJ$14)*$BJ$13/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BA31" s="1" t="n">
+        <f aca="false">(AW31/$BJ$15/$BN$15)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BB31" s="1"/>
+      <c r="BC31" s="1" t="n">
+        <f aca="false">SUM(AY21:AY23)</f>
+        <v>1239725.50666036</v>
+      </c>
+      <c r="BD31" s="1" t="n">
+        <f aca="false">SUM(AZ21:AZ23)</f>
+        <v>1630000</v>
+      </c>
+      <c r="BE31" s="1" t="n">
+        <f aca="false">SUM(BA24:BA29)</f>
+        <v>294066.739345721</v>
+      </c>
+      <c r="BF31" s="1"/>
+      <c r="BG31" s="1"/>
+      <c r="BH31" s="1"/>
+      <c r="BI31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
@@ -72114,10 +72860,16 @@
       <c r="AJ32" s="2"/>
       <c r="AM32" s="7"/>
       <c r="AN32" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM32^$AZ$3</f>
+        <f aca="false">$BJ$2*$BJ$8*AM32^$BJ$3</f>
         <v>0</v>
       </c>
       <c r="AT32" s="10"/>
+      <c r="AW32" s="1" t="n">
+        <f aca="false">AJ32*M32*AS32*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="BA32" s="1"/>
+      <c r="BB32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -72225,12 +72977,12 @@
         <v>296.419992254182</v>
       </c>
       <c r="AM33" s="7" t="n">
-        <f aca="false">AJ33*M33/X33/$AZ$5</f>
+        <f aca="false">AJ33*M33/X33/$BJ$5</f>
         <v>201.022929543821</v>
       </c>
       <c r="AN33" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM33^$AZ$3</f>
-        <v>4.07206707812965</v>
+        <f aca="false">$BJ$2*$BJ$8*AM33^$BJ$3</f>
+        <v>4.07206707812958</v>
       </c>
       <c r="AQ33" s="1" t="n">
         <v>5</v>
@@ -72238,20 +72990,37 @@
       <c r="AR33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS33" s="13" t="n">
+      <c r="AS33" s="19" t="n">
         <v>54</v>
       </c>
       <c r="AT33" s="10" t="n">
-        <f aca="false">$AZ$6*AQ33</f>
+        <f aca="false">$BJ$6*AQ33</f>
         <v>1.5</v>
       </c>
       <c r="AU33" s="11" t="n">
-        <f aca="false">SUMPRODUCT(AZ11*AQ33:AQ46,AS33:AS46) / SUM(AS33:AS46)</f>
+        <f aca="false">SUMPRODUCT(BJ11*AQ33:AQ46,AS33:AS46) / SUM(AS33:AS46)</f>
         <v>25.3203176704169</v>
       </c>
       <c r="AV33" s="1" t="s">
-        <v>924</v>
-      </c>
+        <v>932</v>
+      </c>
+      <c r="AW33" s="1" t="n">
+        <f aca="false">AJ33*M33*AS33*1000/$BJ$17</f>
+        <v>2174530370.39723</v>
+      </c>
+      <c r="AY33" s="1" t="n">
+        <f aca="false">(AW33/$BJ$14)*$BJ$13/1000</f>
+        <v>372785.155728798</v>
+      </c>
+      <c r="AZ33" s="1" t="n">
+        <f aca="false">AS33*AQ33*1000</f>
+        <v>270000</v>
+      </c>
+      <c r="BA33" s="1" t="n">
+        <f aca="false">(AW33/$BJ$15/$BN$15)/1000</f>
+        <v>78605.3438017499</v>
+      </c>
+      <c r="BB33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -72359,12 +73128,12 @@
         <v>178.865181190896</v>
       </c>
       <c r="AM34" s="7" t="n">
-        <f aca="false">AJ34*M34/X34/$AZ$5</f>
+        <f aca="false">AJ34*M34/X34/$BJ$5</f>
         <v>55.933416020056</v>
       </c>
       <c r="AN34" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM34^$AZ$3</f>
-        <v>1.07909051102227</v>
+        <f aca="false">$BJ$2*$BJ$8*AM34^$BJ$3</f>
+        <v>1.07909051102226</v>
       </c>
       <c r="AQ34" s="1" t="n">
         <v>4</v>
@@ -72372,17 +73141,30 @@
       <c r="AR34" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS34" s="13" t="n">
+      <c r="AS34" s="19" t="n">
         <v>442</v>
       </c>
       <c r="AT34" s="10" t="n">
-        <f aca="false">$AZ$6*AQ34</f>
+        <f aca="false">$BJ$6*AQ34</f>
         <v>1.2</v>
       </c>
       <c r="AU34" s="1" t="n">
         <f aca="false">MEDIAN(AQ33:AQ46)</f>
         <v>11</v>
       </c>
+      <c r="AW34" s="1" t="n">
+        <f aca="false">AJ34*M34*AS34*1000/$BJ$17</f>
+        <v>4952445821.33224</v>
+      </c>
+      <c r="AY34" s="1" t="n">
+        <f aca="false">(AW34/$BJ$14)*$BJ$13/1000</f>
+        <v>849010.118173942</v>
+      </c>
+      <c r="BA34" s="1" t="n">
+        <f aca="false">(AW34/$BJ$15/$BN$15)/1000</f>
+        <v>179021.968028089</v>
+      </c>
+      <c r="BB34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -72490,12 +73272,12 @@
         <v>227.426391463863</v>
       </c>
       <c r="AM35" s="7" t="n">
-        <f aca="false">AJ35*M35/X35/$AZ$5</f>
+        <f aca="false">AJ35*M35/X35/$BJ$5</f>
         <v>87.6468075211084</v>
       </c>
       <c r="AN35" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM35^$AZ$3</f>
-        <v>1.72012501561655</v>
+        <f aca="false">$BJ$2*$BJ$8*AM35^$BJ$3</f>
+        <v>1.72012501561652</v>
       </c>
       <c r="AQ35" s="1" t="n">
         <v>2</v>
@@ -72503,13 +73285,30 @@
       <c r="AR35" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS35" s="13" t="n">
+      <c r="AS35" s="19" t="n">
         <v>388</v>
       </c>
       <c r="AT35" s="10" t="n">
-        <f aca="false">$AZ$6*AQ35</f>
+        <f aca="false">$BJ$6*AQ35</f>
         <v>0.6</v>
       </c>
+      <c r="AW35" s="1" t="n">
+        <f aca="false">AJ35*M35*AS35*1000/$BJ$17</f>
+        <v>6812302858.80727</v>
+      </c>
+      <c r="AY35" s="1" t="n">
+        <f aca="false">(AW35/$BJ$14)*$BJ$13/1000</f>
+        <v>1167850.04093932</v>
+      </c>
+      <c r="AZ35" s="1" t="n">
+        <f aca="false">AS35*AQ35*1000</f>
+        <v>776000</v>
+      </c>
+      <c r="BA35" s="1" t="n">
+        <f aca="false">(AW35/$BJ$15/$BN$15)/1000</f>
+        <v>246252.439417699</v>
+      </c>
+      <c r="BB35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -72617,12 +73416,12 @@
         <v>201.142995602393</v>
       </c>
       <c r="AM36" s="7" t="n">
-        <f aca="false">AJ36*M36/X36/$AZ$5</f>
+        <f aca="false">AJ36*M36/X36/$BJ$5</f>
         <v>127.30599925874</v>
       </c>
       <c r="AN36" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM36^$AZ$3</f>
-        <v>2.53427520839856</v>
+        <f aca="false">$BJ$2*$BJ$8*AM36^$BJ$3</f>
+        <v>2.53427520839852</v>
       </c>
       <c r="AQ36" s="1" t="n">
         <v>9</v>
@@ -72630,14 +73429,28 @@
       <c r="AR36" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS36" s="13" t="n">
+      <c r="AS36" s="19" t="n">
         <f aca="false">356/2</f>
         <v>178</v>
       </c>
       <c r="AT36" s="10" t="n">
-        <f aca="false">$AZ$6*AQ36</f>
+        <f aca="false">$BJ$6*AQ36</f>
         <v>2.7</v>
       </c>
+      <c r="AW36" s="1" t="n">
+        <f aca="false">AJ36*M36*AS36*1000/$BJ$17</f>
+        <v>4539363825.98509</v>
+      </c>
+      <c r="AY36" s="1" t="n">
+        <f aca="false">(AW36/$BJ$14)*$BJ$13/1000</f>
+        <v>778194.443184716</v>
+      </c>
+      <c r="AZ36" s="1"/>
+      <c r="BA36" s="1" t="n">
+        <f aca="false">(AW36/$BJ$15/$BN$15)/1000</f>
+        <v>164089.800280694</v>
+      </c>
+      <c r="BB36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
@@ -72745,12 +73558,12 @@
         <v>145.878451592495</v>
       </c>
       <c r="AM37" s="7" t="n">
-        <f aca="false">AJ37*M37/X37/$AZ$5</f>
+        <f aca="false">AJ37*M37/X37/$BJ$5</f>
         <v>456.920953356336</v>
       </c>
       <c r="AN37" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM37^$AZ$3</f>
-        <v>9.55007061512657</v>
+        <f aca="false">$BJ$2*$BJ$8*AM37^$BJ$3</f>
+        <v>9.55007061512637</v>
       </c>
       <c r="AQ37" s="1" t="n">
         <v>32</v>
@@ -72758,14 +73571,28 @@
       <c r="AR37" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS37" s="13" t="n">
+      <c r="AS37" s="19" t="n">
         <f aca="false">586/2</f>
         <v>293</v>
       </c>
       <c r="AT37" s="10" t="n">
-        <f aca="false">$AZ$6*AQ37</f>
+        <f aca="false">$BJ$6*AQ37</f>
         <v>9.6</v>
       </c>
+      <c r="AW37" s="1" t="n">
+        <f aca="false">AJ37*M37*AS37*1000/$BJ$17</f>
+        <v>26818520451.9898</v>
+      </c>
+      <c r="AY37" s="1" t="n">
+        <f aca="false">(AW37/$BJ$14)*$BJ$13/1000</f>
+        <v>4597565.73612936</v>
+      </c>
+      <c r="AZ37" s="1"/>
+      <c r="BA37" s="1" t="n">
+        <f aca="false">(AW37/$BJ$15/$BN$15)/1000</f>
+        <v>969441.056828206</v>
+      </c>
+      <c r="BB37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
@@ -72873,12 +73700,12 @@
         <v>153.267512797817</v>
       </c>
       <c r="AM38" s="7" t="n">
-        <f aca="false">AJ38*M38/X38/$AZ$5</f>
+        <f aca="false">AJ38*M38/X38/$BJ$5</f>
         <v>71.8947371768747</v>
       </c>
       <c r="AN38" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM38^$AZ$3</f>
-        <v>1.40036270814386</v>
+        <f aca="false">$BJ$2*$BJ$8*AM38^$BJ$3</f>
+        <v>1.40036270814384</v>
       </c>
       <c r="AQ38" s="1" t="n">
         <v>8</v>
@@ -72886,13 +73713,27 @@
       <c r="AR38" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS38" s="13" t="n">
+      <c r="AS38" s="19" t="n">
         <v>412</v>
       </c>
       <c r="AT38" s="10" t="n">
-        <f aca="false">$AZ$6*AQ38</f>
+        <f aca="false">$BJ$6*AQ38</f>
         <v>2.4</v>
       </c>
+      <c r="AW38" s="1" t="n">
+        <f aca="false">AJ38*M38*AS38*1000/$BJ$17</f>
+        <v>5933629654.13184</v>
+      </c>
+      <c r="AY38" s="1" t="n">
+        <f aca="false">(AW38/$BJ$14)*$BJ$13/1000</f>
+        <v>1017216.90566616</v>
+      </c>
+      <c r="AZ38" s="1"/>
+      <c r="BA38" s="1" t="n">
+        <f aca="false">(AW38/$BJ$15/$BN$15)/1000</f>
+        <v>214489.99071468</v>
+      </c>
+      <c r="BB38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
@@ -73000,12 +73841,12 @@
         <v>127.131247634543</v>
       </c>
       <c r="AM39" s="7" t="n">
-        <f aca="false">AJ39*M39/X39/$AZ$5</f>
+        <f aca="false">AJ39*M39/X39/$BJ$5</f>
         <v>83.2207000907001</v>
       </c>
       <c r="AN39" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM39^$AZ$3</f>
-        <v>1.63003608969291</v>
+        <f aca="false">$BJ$2*$BJ$8*AM39^$BJ$3</f>
+        <v>1.63003608969289</v>
       </c>
       <c r="AQ39" s="1" t="n">
         <v>9</v>
@@ -73013,13 +73854,27 @@
       <c r="AR39" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS39" s="13" t="n">
+      <c r="AS39" s="19" t="n">
         <v>146</v>
       </c>
       <c r="AT39" s="10" t="n">
-        <f aca="false">$AZ$6*AQ39</f>
+        <f aca="false">$BJ$6*AQ39</f>
         <v>2.7</v>
       </c>
+      <c r="AW39" s="1" t="n">
+        <f aca="false">AJ39*M39*AS39*1000/$BJ$17</f>
+        <v>2433942649.09344</v>
+      </c>
+      <c r="AY39" s="1" t="n">
+        <f aca="false">(AW39/$BJ$14)*$BJ$13/1000</f>
+        <v>417256.848572557</v>
+      </c>
+      <c r="AZ39" s="1"/>
+      <c r="BA39" s="1" t="n">
+        <f aca="false">(AW39/$BJ$15/$BN$15)/1000</f>
+        <v>87982.6289530197</v>
+      </c>
+      <c r="BB39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
@@ -73127,12 +73982,12 @@
         <v>132.799902301287</v>
       </c>
       <c r="AM40" s="7" t="n">
-        <f aca="false">AJ40*M40/X40/$AZ$5</f>
+        <f aca="false">AJ40*M40/X40/$BJ$5</f>
         <v>103.440356333057</v>
       </c>
       <c r="AN40" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM40^$AZ$3</f>
-        <v>2.04294821600913</v>
+        <f aca="false">$BJ$2*$BJ$8*AM40^$BJ$3</f>
+        <v>2.0429482160091</v>
       </c>
       <c r="AQ40" s="1" t="n">
         <v>10</v>
@@ -73140,13 +73995,27 @@
       <c r="AR40" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS40" s="13" t="n">
+      <c r="AS40" s="19" t="n">
         <v>309</v>
       </c>
       <c r="AT40" s="10" t="n">
-        <f aca="false">$AZ$6*AQ40</f>
+        <f aca="false">$BJ$6*AQ40</f>
         <v>3</v>
       </c>
+      <c r="AW40" s="1" t="n">
+        <f aca="false">AJ40*M40*AS40*1000/$BJ$17</f>
+        <v>6402868866.41419</v>
+      </c>
+      <c r="AY40" s="1" t="n">
+        <f aca="false">(AW40/$BJ$14)*$BJ$13/1000</f>
+        <v>1097659.75217962</v>
+      </c>
+      <c r="AZ40" s="1"/>
+      <c r="BA40" s="1" t="n">
+        <f aca="false">(AW40/$BJ$15/$BN$15)/1000</f>
+        <v>231452.140385636</v>
+      </c>
+      <c r="BB40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
@@ -73254,12 +74123,12 @@
         <v>95.8179222700966</v>
       </c>
       <c r="AM41" s="7" t="n">
-        <f aca="false">AJ41*M41/X41/$AZ$5</f>
+        <f aca="false">AJ41*M41/X41/$BJ$5</f>
         <v>80.0784617650687</v>
       </c>
       <c r="AN41" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM41^$AZ$3</f>
-        <v>1.56618928098836</v>
+        <f aca="false">$BJ$2*$BJ$8*AM41^$BJ$3</f>
+        <v>1.56618928098834</v>
       </c>
       <c r="AQ41" s="1" t="n">
         <v>12</v>
@@ -73267,12 +74136,29 @@
       <c r="AR41" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS41" s="13" t="n">
+      <c r="AS41" s="19" t="n">
         <v>244</v>
       </c>
       <c r="AT41" s="10" t="n">
-        <f aca="false">$AZ$6*AQ41</f>
+        <f aca="false">$BJ$6*AQ41</f>
         <v>3.6</v>
+      </c>
+      <c r="AW41" s="1" t="n">
+        <f aca="false">AJ41*M41*AS41*1000/$BJ$17</f>
+        <v>3914097759.3756</v>
+      </c>
+      <c r="AY41" s="1" t="n">
+        <f aca="false">(AW41/$BJ$14)*$BJ$13/1000</f>
+        <v>671003.524544949</v>
+      </c>
+      <c r="AZ41" s="1"/>
+      <c r="BA41" s="1" t="n">
+        <f aca="false">(AW41/$BJ$15/$BN$15)/1000</f>
+        <v>141487.561745654</v>
+      </c>
+      <c r="BB41" s="1"/>
+      <c r="BG41" s="1" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -73381,12 +74267,12 @@
         <v>57.436839767136</v>
       </c>
       <c r="AM42" s="7" t="n">
-        <f aca="false">AJ42*M42/X42/$AZ$5</f>
+        <f aca="false">AJ42*M42/X42/$BJ$5</f>
         <v>125.91834111512</v>
       </c>
       <c r="AN42" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM42^$AZ$3</f>
-        <v>2.5056038928248</v>
+        <f aca="false">$BJ$2*$BJ$8*AM42^$BJ$3</f>
+        <v>2.50560389282476</v>
       </c>
       <c r="AQ42" s="1" t="n">
         <v>19</v>
@@ -73394,12 +74280,35 @@
       <c r="AR42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS42" s="13" t="n">
+      <c r="AS42" s="19" t="n">
         <v>85</v>
       </c>
       <c r="AT42" s="10" t="n">
-        <f aca="false">$AZ$6*AQ42</f>
+        <f aca="false">$BJ$6*AQ42</f>
         <v>5.7</v>
+      </c>
+      <c r="AW42" s="1" t="n">
+        <f aca="false">AJ42*M42*AS42*1000/$BJ$17</f>
+        <v>2144045705.99366</v>
+      </c>
+      <c r="AY42" s="1" t="n">
+        <f aca="false">(AW42/$BJ$14)*$BJ$13/1000</f>
+        <v>367559.093806772</v>
+      </c>
+      <c r="AZ42" s="1"/>
+      <c r="BA42" s="1" t="n">
+        <f aca="false">(AW42/$BJ$15/$BN$15)/1000</f>
+        <v>77503.3782653082</v>
+      </c>
+      <c r="BB42" s="1"/>
+      <c r="BC42" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="BD42" s="13"/>
+      <c r="BE42" s="13"/>
+      <c r="BG42" s="14" t="n">
+        <f aca="false">(SUM(AW33:AW42)+AW45+AW46)/1000</f>
+        <v>98098936.4789487</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -73512,12 +74421,12 @@
         <v>72.7323706816538</v>
       </c>
       <c r="AM43" s="7" t="n">
-        <f aca="false">AJ43*M43/X43/$AZ$5</f>
+        <f aca="false">AJ43*M43/X43/$BJ$5</f>
         <v>97.6499421188871</v>
       </c>
       <c r="AN43" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM43^$AZ$3</f>
-        <v>1.92435618467017</v>
+        <f aca="false">$BJ$2*$BJ$8*AM43^$BJ$3</f>
+        <v>1.92435618467014</v>
       </c>
       <c r="AQ43" s="1" t="n">
         <v>17</v>
@@ -73525,12 +74434,25 @@
       <c r="AR43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS43" s="13" t="n">
+      <c r="AS43" s="19" t="n">
         <v>0</v>
       </c>
       <c r="AT43" s="10" t="n">
-        <f aca="false">$AZ$6*AQ43</f>
+        <f aca="false">$BJ$6*AQ43</f>
         <v>5.1</v>
+      </c>
+      <c r="AY43" s="1" t="n">
+        <f aca="false">(AW43/$BJ$14)*$BJ$13/1000</f>
+        <v>0</v>
+      </c>
+      <c r="AZ43" s="1"/>
+      <c r="BA43" s="1" t="n">
+        <f aca="false">(AW43/$BJ$15/$BN$15)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BB43" s="1"/>
+      <c r="BG43" s="1" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -73643,12 +74565,12 @@
         <v>71.3784162731017</v>
       </c>
       <c r="AM44" s="7" t="n">
-        <f aca="false">AJ44*M44/X44/$AZ$5</f>
+        <f aca="false">AJ44*M44/X44/$BJ$5</f>
         <v>95.8321329592569</v>
       </c>
       <c r="AN44" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM44^$AZ$3</f>
-        <v>1.88718062833286</v>
+        <f aca="false">$BJ$2*$BJ$8*AM44^$BJ$3</f>
+        <v>1.88718062833283</v>
       </c>
       <c r="AQ44" s="1" t="n">
         <v>17</v>
@@ -73656,12 +74578,36 @@
       <c r="AR44" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS44" s="13" t="n">
+      <c r="AS44" s="19" t="n">
         <v>0</v>
       </c>
       <c r="AT44" s="10" t="n">
-        <f aca="false">$AZ$6*AQ44</f>
+        <f aca="false">$BJ$6*AQ44</f>
         <v>5.1</v>
+      </c>
+      <c r="AY44" s="1" t="n">
+        <f aca="false">(AW44/$BJ$14)*$BJ$13/1000</f>
+        <v>0</v>
+      </c>
+      <c r="AZ44" s="1"/>
+      <c r="BA44" s="1" t="n">
+        <f aca="false">(AW44/$BJ$15/$BN$15)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="BB44" s="1"/>
+      <c r="BC44" s="12" t="s">
+        <v>946</v>
+      </c>
+      <c r="BD44" s="8" t="n">
+        <f aca="false">(AY33+SUM(AY36:AY42)+AY46)/SUM(AY33:AY46)</f>
+        <v>0.771542772743223</v>
+      </c>
+      <c r="BE44" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BG44" s="16" t="n">
+        <f aca="false">BD44*SUM(AW33:AW46)/1000</f>
+        <v>75687525.4541294</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -73770,12 +74716,12 @@
         <v>154.688577389639</v>
       </c>
       <c r="AM45" s="7" t="n">
-        <f aca="false">AJ45*M45/X45/$AZ$5</f>
+        <f aca="false">AJ45*M45/X45/$BJ$5</f>
         <v>298.58456834879</v>
       </c>
       <c r="AN45" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM45^$AZ$3</f>
-        <v>6.14027555330027</v>
+        <f aca="false">$BJ$2*$BJ$8*AM45^$BJ$3</f>
+        <v>6.14027555330016</v>
       </c>
       <c r="AQ45" s="1" t="n">
         <v>16</v>
@@ -73783,14 +74729,31 @@
       <c r="AR45" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS45" s="13" t="n">
+      <c r="AS45" s="19" t="n">
         <f aca="false">356/2</f>
         <v>178</v>
       </c>
       <c r="AT45" s="10" t="n">
-        <f aca="false">$AZ$6*AQ45</f>
+        <f aca="false">$BJ$6*AQ45</f>
         <v>4.8</v>
       </c>
+      <c r="AW45" s="1" t="n">
+        <f aca="false">AJ45*M45*AS45*1000/$BJ$17</f>
+        <v>10646662344.6799</v>
+      </c>
+      <c r="AY45" s="1" t="n">
+        <f aca="false">(AW45/$BJ$14)*$BJ$13/1000</f>
+        <v>1825183.83471848</v>
+      </c>
+      <c r="AZ45" s="1" t="n">
+        <f aca="false">AS45*AQ45*1000</f>
+        <v>2848000</v>
+      </c>
+      <c r="BA45" s="1" t="n">
+        <f aca="false">(AW45/$BJ$15/$BN$15)/1000</f>
+        <v>384857.60665271</v>
+      </c>
+      <c r="BB45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
@@ -73898,12 +74861,12 @@
         <v>132.366139946455</v>
       </c>
       <c r="AM46" s="7" t="n">
-        <f aca="false">AJ46*M46/X46/$AZ$5</f>
+        <f aca="false">AJ46*M46/X46/$BJ$5</f>
         <v>363.351016591755</v>
       </c>
       <c r="AN46" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM46^$AZ$3</f>
-        <v>7.52831212772735</v>
+        <f aca="false">$BJ$2*$BJ$8*AM46^$BJ$3</f>
+        <v>7.5283121277272</v>
       </c>
       <c r="AQ46" s="1" t="n">
         <v>32</v>
@@ -73911,22 +74874,66 @@
       <c r="AR46" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS46" s="13" t="n">
+      <c r="AS46" s="19" t="n">
         <f aca="false">586/2</f>
         <v>293</v>
       </c>
       <c r="AT46" s="10" t="n">
-        <f aca="false">$AZ$6*AQ46</f>
+        <f aca="false">$BJ$6*AQ46</f>
         <v>9.6</v>
       </c>
+      <c r="AW46" s="1" t="n">
+        <f aca="false">AJ46*M46*AS46*1000/$BJ$17</f>
+        <v>21326526170.7485</v>
+      </c>
+      <c r="AY46" s="1" t="n">
+        <f aca="false">(AW46/$BJ$14)*$BJ$13/1000</f>
+        <v>3656059.48205934</v>
+      </c>
+      <c r="BA46" s="1" t="n">
+        <f aca="false">(AW46/$BJ$15/$BN$15)/1000</f>
+        <v>770915.386866946</v>
+      </c>
+      <c r="BB46" s="1"/>
+      <c r="BC46" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD46" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="BE46" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="BF46" s="1"/>
+      <c r="BG46" s="1"/>
+      <c r="BH46" s="1"/>
+      <c r="BI46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AM47" s="7"/>
       <c r="AN47" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM47^$AZ$3</f>
+        <f aca="false">$BJ$2*$BJ$8*AM47^$BJ$3</f>
         <v>0</v>
       </c>
       <c r="AT47" s="10"/>
+      <c r="BA47" s="1"/>
+      <c r="BB47" s="1"/>
+      <c r="BC47" s="1" t="n">
+        <f aca="false">AY33+AY35</f>
+        <v>1540635.19666812</v>
+      </c>
+      <c r="BD47" s="1" t="n">
+        <f aca="false">AZ33+AZ35+AZ45</f>
+        <v>3894000</v>
+      </c>
+      <c r="BE47" s="1" t="n">
+        <f aca="false">SUM(BA48:BA57)</f>
+        <v>1138724.52400189</v>
+      </c>
+      <c r="BF47" s="1"/>
+      <c r="BG47" s="1"/>
+      <c r="BH47" s="1"/>
+      <c r="BI47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
@@ -74034,12 +75041,12 @@
         <v>139.394347636144</v>
       </c>
       <c r="AM48" s="7" t="n">
-        <f aca="false">AJ48*M48/X48/$AZ$5</f>
+        <f aca="false">AJ48*M48/X48/$BJ$5</f>
         <v>115.729401330749</v>
       </c>
       <c r="AN48" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM48^$AZ$3</f>
-        <v>2.29546103865102</v>
+        <f aca="false">$BJ$2*$BJ$8*AM48^$BJ$3</f>
+        <v>2.29546103865099</v>
       </c>
       <c r="AQ48" s="1" t="n">
         <v>11</v>
@@ -74047,20 +75054,33 @@
       <c r="AR48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS48" s="13" t="n">
+      <c r="AS48" s="19" t="n">
         <v>0.6</v>
       </c>
       <c r="AT48" s="10" t="n">
-        <f aca="false">$AZ$6*AQ48</f>
+        <f aca="false">$BJ$6*AQ48</f>
         <v>3.3</v>
       </c>
       <c r="AU48" s="11" t="n">
-        <f aca="false">SUMPRODUCT(AZ11*AQ48:AQ58,AS48:AS58) / SUM(AS48:AS58)</f>
+        <f aca="false">SUMPRODUCT(BJ11*AQ48:AQ58,AS48:AS58) / SUM(AS48:AS58)</f>
         <v>124.193195336664</v>
       </c>
       <c r="AV48" s="2" t="s">
-        <v>924</v>
-      </c>
+        <v>932</v>
+      </c>
+      <c r="AW48" s="1" t="n">
+        <f aca="false">AJ48*M48*AS48*1000/$BJ$17</f>
+        <v>13909806.1274615</v>
+      </c>
+      <c r="AY48" s="1" t="n">
+        <f aca="false">(AW48/$BJ$14)*$BJ$13/1000</f>
+        <v>2384.59269825508</v>
+      </c>
+      <c r="BA48" s="1" t="n">
+        <f aca="false">(AW48/$BJ$15/$BN$15)/1000</f>
+        <v>502.814358332032</v>
+      </c>
+      <c r="BB48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
@@ -74168,12 +75188,12 @@
         <v>173.706708954303</v>
       </c>
       <c r="AM49" s="7" t="n">
-        <f aca="false">AJ49*M49/X49/$AZ$5</f>
+        <f aca="false">AJ49*M49/X49/$BJ$5</f>
         <v>258.042446375449</v>
       </c>
       <c r="AN49" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM49^$AZ$3</f>
-        <v>5.27709923493732</v>
+        <f aca="false">$BJ$2*$BJ$8*AM49^$BJ$3</f>
+        <v>5.27709923493722</v>
       </c>
       <c r="AQ49" s="1" t="n">
         <v>15</v>
@@ -74181,17 +75201,34 @@
       <c r="AR49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS49" s="13" t="n">
+      <c r="AS49" s="19" t="n">
         <v>28.7</v>
       </c>
       <c r="AT49" s="10" t="n">
-        <f aca="false">$AZ$6*AQ49</f>
+        <f aca="false">$BJ$6*AQ49</f>
         <v>4.5</v>
       </c>
-      <c r="AU49" s="14" t="n">
+      <c r="AU49" s="12" t="n">
         <f aca="false">MEDIAN(AQ48:AQ59)</f>
         <v>32</v>
       </c>
+      <c r="AW49" s="1" t="n">
+        <f aca="false">AJ49*M49*AS49*1000/$BJ$17</f>
+        <v>1483539681.72537</v>
+      </c>
+      <c r="AY49" s="1" t="n">
+        <f aca="false">(AW49/$BJ$14)*$BJ$13/1000</f>
+        <v>254326.901482097</v>
+      </c>
+      <c r="AZ49" s="1" t="n">
+        <f aca="false">AS49*AQ49*1000</f>
+        <v>430500</v>
+      </c>
+      <c r="BA49" s="1" t="n">
+        <f aca="false">(AW49/$BJ$15/$BN$15)/1000</f>
+        <v>53627.2789348346</v>
+      </c>
+      <c r="BB49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
@@ -74299,12 +75336,12 @@
         <v>170.283418701034</v>
       </c>
       <c r="AM50" s="7" t="n">
-        <f aca="false">AJ50*M50/X50/$AZ$5</f>
+        <f aca="false">AJ50*M50/X50/$BJ$5</f>
         <v>273.186421573721</v>
       </c>
       <c r="AN50" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM50^$AZ$3</f>
-        <v>5.59896259944886</v>
+        <f aca="false">$BJ$2*$BJ$8*AM50^$BJ$3</f>
+        <v>5.59896259944876</v>
       </c>
       <c r="AQ50" s="1" t="n">
         <v>20</v>
@@ -74312,13 +75349,26 @@
       <c r="AR50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS50" s="13" t="n">
+      <c r="AS50" s="19" t="n">
         <v>7.4</v>
       </c>
       <c r="AT50" s="10" t="n">
-        <f aca="false">$AZ$6*AQ50</f>
+        <f aca="false">$BJ$6*AQ50</f>
         <v>6</v>
       </c>
+      <c r="AW50" s="1" t="n">
+        <f aca="false">AJ50*M50*AS50*1000/$BJ$17</f>
+        <v>404964495.714034</v>
+      </c>
+      <c r="AY50" s="1" t="n">
+        <f aca="false">(AW50/$BJ$14)*$BJ$13/1000</f>
+        <v>69424.071815476</v>
+      </c>
+      <c r="BA50" s="1" t="n">
+        <f aca="false">(AW50/$BJ$15/$BN$15)/1000</f>
+        <v>14638.7348029032</v>
+      </c>
+      <c r="BB50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
@@ -74426,12 +75476,12 @@
         <v>148.512073375188</v>
       </c>
       <c r="AM51" s="7" t="n">
-        <f aca="false">AJ51*M51/X51/$AZ$5</f>
+        <f aca="false">AJ51*M51/X51/$BJ$5</f>
         <v>577.903737776482</v>
       </c>
       <c r="AN51" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM51^$AZ$3</f>
-        <v>12.1873867356033</v>
+        <f aca="false">$BJ$2*$BJ$8*AM51^$BJ$3</f>
+        <v>12.187386735603</v>
       </c>
       <c r="AQ51" s="1" t="n">
         <v>48</v>
@@ -74439,13 +75489,26 @@
       <c r="AR51" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="AS51" s="13" t="n">
+      <c r="AS51" s="19" t="n">
         <v>17.3</v>
       </c>
       <c r="AT51" s="10" t="n">
-        <f aca="false">$AZ$6*AQ51</f>
+        <f aca="false">$BJ$6*AQ51</f>
         <v>14.4</v>
       </c>
+      <c r="AW51" s="1" t="n">
+        <f aca="false">AJ51*M51*AS51*1000/$BJ$17</f>
+        <v>2002754547.59768</v>
+      </c>
+      <c r="AY51" s="1" t="n">
+        <f aca="false">(AW51/$BJ$14)*$BJ$13/1000</f>
+        <v>343337.198724144</v>
+      </c>
+      <c r="BA51" s="1" t="n">
+        <f aca="false">(AW51/$BJ$15/$BN$15)/1000</f>
+        <v>72395.9581836863</v>
+      </c>
+      <c r="BB51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
@@ -74553,12 +75616,12 @@
         <v>126.166392410234</v>
       </c>
       <c r="AM52" s="7" t="n">
-        <f aca="false">AJ52*M52/X52/$AZ$5</f>
+        <f aca="false">AJ52*M52/X52/$BJ$5</f>
         <v>419.544299886684</v>
       </c>
       <c r="AN52" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM52^$AZ$3</f>
-        <v>8.74037759835763</v>
+        <f aca="false">$BJ$2*$BJ$8*AM52^$BJ$3</f>
+        <v>8.74037759835746</v>
       </c>
       <c r="AQ52" s="1" t="n">
         <v>48</v>
@@ -74566,12 +75629,28 @@
       <c r="AR52" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="AS52" s="13" t="n">
+      <c r="AS52" s="19" t="n">
         <v>34</v>
       </c>
       <c r="AT52" s="10" t="n">
-        <f aca="false">$AZ$6*AQ52</f>
+        <f aca="false">$BJ$6*AQ52</f>
         <v>14.4</v>
+      </c>
+      <c r="AW52" s="1" t="n">
+        <f aca="false">AJ52*M52*AS52*1000/$BJ$17</f>
+        <v>2857477780.21879</v>
+      </c>
+      <c r="AY52" s="1" t="n">
+        <f aca="false">(AW52/$BJ$14)*$BJ$13/1000</f>
+        <v>489864.53065535</v>
+      </c>
+      <c r="BA52" s="1" t="n">
+        <f aca="false">(AW52/$BJ$15/$BN$15)/1000</f>
+        <v>103292.658671366</v>
+      </c>
+      <c r="BB52" s="1"/>
+      <c r="BG52" s="1" t="s">
+        <v>936</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -74680,12 +75759,12 @@
         <v>120.098823687048</v>
       </c>
       <c r="AM53" s="7" t="n">
-        <f aca="false">AJ53*M53/X53/$AZ$5</f>
+        <f aca="false">AJ53*M53/X53/$BJ$5</f>
         <v>1376.36377640468</v>
       </c>
       <c r="AN53" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM53^$AZ$3</f>
-        <v>30.0025261528844</v>
+        <f aca="false">$BJ$2*$BJ$8*AM53^$BJ$3</f>
+        <v>30.0025261528837</v>
       </c>
       <c r="AQ53" s="1" t="n">
         <v>189</v>
@@ -74693,12 +75772,34 @@
       <c r="AR53" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="AS53" s="13" t="n">
+      <c r="AS53" s="19" t="n">
         <v>50.1</v>
       </c>
       <c r="AT53" s="10" t="n">
-        <f aca="false">$AZ$6*AQ53</f>
+        <f aca="false">$BJ$6*AQ53</f>
         <v>56.7</v>
+      </c>
+      <c r="AW53" s="1" t="n">
+        <f aca="false">AJ53*M53*AS53*1000/$BJ$17</f>
+        <v>13813288424.4389</v>
+      </c>
+      <c r="AY53" s="1" t="n">
+        <f aca="false">(AW53/$BJ$14)*$BJ$13/1000</f>
+        <v>2368046.42810788</v>
+      </c>
+      <c r="BA53" s="1" t="n">
+        <f aca="false">(AW53/$BJ$15/$BN$15)/1000</f>
+        <v>499325.417762459</v>
+      </c>
+      <c r="BB53" s="1"/>
+      <c r="BC53" s="13" t="s">
+        <v>938</v>
+      </c>
+      <c r="BD53" s="13"/>
+      <c r="BE53" s="13"/>
+      <c r="BG53" s="14" t="n">
+        <f aca="false">SUM(AW48:AW58)/1000</f>
+        <v>55740837.0094373</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -74807,12 +75908,12 @@
         <v>121.215361012558</v>
       </c>
       <c r="AM54" s="7" t="n">
-        <f aca="false">AJ54*M54/X54/$AZ$5</f>
+        <f aca="false">AJ54*M54/X54/$BJ$5</f>
         <v>2404.06825907309</v>
       </c>
       <c r="AN54" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM54^$AZ$3</f>
-        <v>53.5311337095793</v>
+        <f aca="false">$BJ$2*$BJ$8*AM54^$BJ$3</f>
+        <v>53.5311337095779</v>
       </c>
       <c r="AQ54" s="1" t="n">
         <v>254</v>
@@ -74820,12 +75921,28 @@
       <c r="AR54" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="AS54" s="13" t="n">
+      <c r="AS54" s="19" t="n">
         <v>15</v>
       </c>
       <c r="AT54" s="10" t="n">
-        <f aca="false">$AZ$6*AQ54</f>
+        <f aca="false">$BJ$6*AQ54</f>
         <v>76.2</v>
+      </c>
+      <c r="AW54" s="1" t="n">
+        <f aca="false">AJ54*M54*AS54*1000/$BJ$17</f>
+        <v>7223774385.84524</v>
+      </c>
+      <c r="AY54" s="1" t="n">
+        <f aca="false">(AW54/$BJ$14)*$BJ$13/1000</f>
+        <v>1238389.62933643</v>
+      </c>
+      <c r="BA54" s="1" t="n">
+        <f aca="false">(AW54/$BJ$15/$BN$15)/1000</f>
+        <v>261126.391645619</v>
+      </c>
+      <c r="BB54" s="1"/>
+      <c r="BG54" s="1" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -74934,12 +76051,12 @@
         <v>110.593123173294</v>
       </c>
       <c r="AM55" s="7" t="n">
-        <f aca="false">AJ55*M55/X55/$AZ$5</f>
+        <f aca="false">AJ55*M55/X55/$BJ$5</f>
         <v>344.012142403415</v>
       </c>
       <c r="AN55" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM55^$AZ$3</f>
-        <v>7.11277999349788</v>
+        <f aca="false">$BJ$2*$BJ$8*AM55^$BJ$3</f>
+        <v>7.11277999349774</v>
       </c>
       <c r="AQ55" s="1" t="n">
         <v>24</v>
@@ -74947,12 +76064,39 @@
       <c r="AR55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS55" s="13" t="n">
+      <c r="AS55" s="19" t="n">
         <v>28.7</v>
       </c>
       <c r="AT55" s="10" t="n">
-        <f aca="false">$AZ$6*AQ55</f>
+        <f aca="false">$BJ$6*AQ55</f>
         <v>7.2</v>
+      </c>
+      <c r="AW55" s="1" t="n">
+        <f aca="false">AJ55*M55*AS55*1000/$BJ$17</f>
+        <v>1977797340.78424</v>
+      </c>
+      <c r="AY55" s="1" t="n">
+        <f aca="false">(AW55/$BJ$14)*$BJ$13/1000</f>
+        <v>339058.72261953</v>
+      </c>
+      <c r="BA55" s="1" t="n">
+        <f aca="false">(AW55/$BJ$15/$BN$15)/1000</f>
+        <v>71493.8002517447</v>
+      </c>
+      <c r="BB55" s="1"/>
+      <c r="BC55" s="12" t="s">
+        <v>946</v>
+      </c>
+      <c r="BD55" s="8" t="n">
+        <f aca="false">(AY48+SUM(AY50:AY57))/SUM(AY48:AY58)</f>
+        <v>0.538528362477375</v>
+      </c>
+      <c r="BE55" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BG55" s="16" t="n">
+        <f aca="false">BD55*SUM(AW48:AW58)/1000</f>
+        <v>30018021.6778105</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -75061,12 +76205,12 @@
         <v>99.9591345069508</v>
       </c>
       <c r="AM56" s="7" t="n">
-        <f aca="false">AJ56*M56/X56/$AZ$5</f>
+        <f aca="false">AJ56*M56/X56/$BJ$5</f>
         <v>310.933944424774</v>
       </c>
       <c r="AN56" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM56^$AZ$3</f>
-        <v>6.40412377267326</v>
+        <f aca="false">$BJ$2*$BJ$8*AM56^$BJ$3</f>
+        <v>6.40412377267314</v>
       </c>
       <c r="AQ56" s="1" t="n">
         <v>24</v>
@@ -75074,13 +76218,26 @@
       <c r="AR56" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS56" s="13" t="n">
+      <c r="AS56" s="19" t="n">
         <v>20.9</v>
       </c>
       <c r="AT56" s="10" t="n">
-        <f aca="false">$AZ$6*AQ56</f>
+        <f aca="false">$BJ$6*AQ56</f>
         <v>7.2</v>
       </c>
+      <c r="AW56" s="1" t="n">
+        <f aca="false">AJ56*M56*AS56*1000/$BJ$17</f>
+        <v>1301788834.77829</v>
+      </c>
+      <c r="AY56" s="1" t="n">
+        <f aca="false">(AW56/$BJ$14)*$BJ$13/1000</f>
+        <v>223168.901251163</v>
+      </c>
+      <c r="BA56" s="1" t="n">
+        <f aca="false">(AW56/$BJ$15/$BN$15)/1000</f>
+        <v>47057.314217384</v>
+      </c>
+      <c r="BB56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
@@ -75188,12 +76345,12 @@
         <v>89.1663146343626</v>
       </c>
       <c r="AM57" s="7" t="n">
-        <f aca="false">AJ57*M57/X57/$AZ$5</f>
+        <f aca="false">AJ57*M57/X57/$BJ$5</f>
         <v>277.361684410693</v>
       </c>
       <c r="AN57" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM57^$AZ$3</f>
-        <v>5.68782314617998</v>
+        <f aca="false">$BJ$2*$BJ$8*AM57^$BJ$3</f>
+        <v>5.68782314617987</v>
       </c>
       <c r="AQ57" s="1" t="n">
         <v>24</v>
@@ -75201,13 +76358,38 @@
       <c r="AR57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS57" s="13" t="n">
+      <c r="AS57" s="19" t="n">
         <v>7.6</v>
       </c>
       <c r="AT57" s="10" t="n">
-        <f aca="false">$AZ$6*AQ57</f>
+        <f aca="false">$BJ$6*AQ57</f>
         <v>7.2</v>
       </c>
+      <c r="AW57" s="1" t="n">
+        <f aca="false">AJ57*M57*AS57*1000/$BJ$17</f>
+        <v>422266062.305944</v>
+      </c>
+      <c r="AY57" s="1" t="n">
+        <f aca="false">(AW57/$BJ$14)*$BJ$13/1000</f>
+        <v>72390.1224552465</v>
+      </c>
+      <c r="BA57" s="1" t="n">
+        <f aca="false">(AW57/$BJ$15/$BN$15)/1000</f>
+        <v>15264.1551735635</v>
+      </c>
+      <c r="BB57" s="1"/>
+      <c r="BC57" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD57" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="BE57" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="BF57" s="1"/>
+      <c r="BG57" s="1"/>
+      <c r="BH57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
@@ -75315,12 +76497,12 @@
         <v>109.110827986217</v>
       </c>
       <c r="AM58" s="7" t="n">
-        <f aca="false">AJ58*M58/X58/$AZ$5</f>
+        <f aca="false">AJ58*M58/X58/$BJ$5</f>
         <v>576.201285409496</v>
       </c>
       <c r="AN58" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM58^$AZ$3</f>
-        <v>12.1501169885898</v>
+        <f aca="false">$BJ$2*$BJ$8*AM58^$BJ$3</f>
+        <v>12.1501169885896</v>
       </c>
       <c r="AQ58" s="1" t="n">
         <v>40</v>
@@ -75328,13 +76510,46 @@
       <c r="AR58" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="AS58" s="13" t="n">
+      <c r="AS58" s="19" t="n">
         <v>210</v>
       </c>
       <c r="AT58" s="10" t="n">
-        <f aca="false">$AZ$6*AQ58</f>
+        <f aca="false">$BJ$6*AQ58</f>
         <v>12</v>
       </c>
+      <c r="AW58" s="1" t="n">
+        <f aca="false">AJ58*M58*AS58*1000/$BJ$17</f>
+        <v>24239275649.9014</v>
+      </c>
+      <c r="AY58" s="1" t="n">
+        <f aca="false">(AW58/$BJ$14)*$BJ$13/1000</f>
+        <v>4155399.37768315</v>
+      </c>
+      <c r="AZ58" s="1" t="n">
+        <f aca="false">AS58*AQ58*1000</f>
+        <v>8400000</v>
+      </c>
+      <c r="BA58" s="1" t="n">
+        <f aca="false">(AW58/$BJ$15/$BN$15)/1000</f>
+        <v>876206.017586147</v>
+      </c>
+      <c r="BB58" s="1"/>
+      <c r="BC58" s="1" t="n">
+        <f aca="false">AY49+AY58</f>
+        <v>4409726.27916525</v>
+      </c>
+      <c r="BD58" s="1" t="n">
+        <f aca="false">AZ49+AZ58</f>
+        <v>8830500</v>
+      </c>
+      <c r="BE58" s="1" t="n">
+        <f aca="false">SUM(BA48:BA57)/1000000</f>
+        <v>1.13872452400189</v>
+      </c>
+      <c r="BF58" s="1"/>
+      <c r="BG58" s="1"/>
+      <c r="BH58" s="1"/>
+      <c r="BI58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
@@ -75442,12 +76657,12 @@
         <v>104.088376160451</v>
       </c>
       <c r="AM59" s="7" t="n">
-        <f aca="false">AJ59*M59/X59/$AZ$5</f>
+        <f aca="false">AJ59*M59/X59/$BJ$5</f>
         <v>833.227972127254</v>
       </c>
       <c r="AN59" s="8" t="n">
-        <f aca="false">$AZ$2*$AZ$8*AM59^$AZ$3</f>
-        <v>17.8187710439887</v>
+        <f aca="false">$BJ$2*$BJ$8*AM59^$BJ$3</f>
+        <v>17.8187710439883</v>
       </c>
       <c r="AQ59" s="1" t="n">
         <v>64</v>
@@ -75455,24 +76670,142 @@
       <c r="AR59" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="AS59" s="13"/>
+      <c r="AS59" s="19"/>
       <c r="AT59" s="10" t="n">
-        <f aca="false">$AZ$6*AQ59</f>
+        <f aca="false">$BJ$6*AQ59</f>
         <v>19.2</v>
       </c>
+      <c r="AW59" s="1" t="n">
+        <f aca="false">AJ59*M59*AS59*1000/$BJ$17</f>
+        <v>0</v>
+      </c>
+      <c r="AY59" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA59" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BD60" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="BE60" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="BG60" s="1" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BD61" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="BE61" s="20" t="s">
+        <v>950</v>
+      </c>
+      <c r="BG61" s="1" t="n">
+        <f aca="false">(BG16+BG28+BG44+BG55)/1000000</f>
+        <v>118.953912614449</v>
+      </c>
+      <c r="BH61" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="BI61" s="0" t="n">
+        <f aca="false">BG61*1000000000/BJ15/BN15</f>
+        <v>4299969007.0615</v>
+      </c>
+      <c r="BJ61" s="0" t="s">
+        <v>956</v>
+      </c>
+      <c r="BK61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AR62" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="AS62" s="1" t="n">
+        <f aca="false">SUMPRODUCT(AQ7:AQ59,AS7:AS59)*1000</f>
+        <v>80628200</v>
+      </c>
+      <c r="AW62" s="11" t="n">
+        <f aca="false">SUM(AW7:AW58)/1000000000</f>
+        <v>241.190212671658</v>
+      </c>
+      <c r="AX62" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="AY62" s="11" t="n">
+        <f aca="false">SUM(AY7:AY59)/1000000</f>
+        <v>41.3478386943115</v>
+      </c>
+      <c r="AZ62" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="BA62" s="1"/>
+      <c r="BB62" s="1"/>
+      <c r="BD62" s="15" t="n">
+        <f aca="false">SUM(BD19:BD58)/AS62</f>
+        <v>0.298710647632816</v>
+      </c>
+      <c r="BE62" s="21" t="n">
+        <f aca="false">(BE58+BE47+BE31+BE19)/1000000</f>
+        <v>1.61763013687897</v>
+      </c>
+      <c r="BF62" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="BI62" s="0" t="n">
+        <f aca="false">BI61/1000000000</f>
+        <v>4.2999690070615</v>
+      </c>
+      <c r="BJ62" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="BK62" s="1"/>
+    </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AY64" s="22" t="s">
+        <v>912</v>
+      </c>
+      <c r="AZ64" s="22"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AY65" s="23" t="s">
+        <v>951</v>
+      </c>
+      <c r="AZ65" s="23" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AY66" s="24" t="n">
+        <f aca="false">(BC19+BC31+BC47+BC58)/1000000</f>
+        <v>18.6538644760328</v>
+      </c>
+      <c r="AZ66" s="24" t="n">
+        <f aca="false">AY62-AY66</f>
+        <v>22.6939742182788</v>
+      </c>
+    </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AW69" s="25" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AW70" s="1" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AW71" s="1" t="s">
+        <v>964</v>
+      </c>
+    </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -75486,6 +76819,13 @@
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="BC14:BE14"/>
+    <mergeCell ref="BC26:BE26"/>
+    <mergeCell ref="BC42:BE42"/>
+    <mergeCell ref="BC53:BE53"/>
+    <mergeCell ref="AY64:AZ64"/>
+  </mergeCells>
   <conditionalFormatting sqref="AM7:AM59">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -75506,6 +76846,9 @@
       <formula>$AT7&lt;$AN7</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="AW69" r:id="rId1" display="601 Twh is in the right order of magnitude as can be seen here : https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/natural-gas/021623-german-gas-consumption-remains-in-critical-range-in-week-6-regulator"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -75527,7 +76870,7 @@
       <selection pane="topLeft" activeCell="S24" activeCellId="0" sqref="S24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.97"/>
@@ -75535,70 +76878,70 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>928</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>929</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>930</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>931</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>932</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>933</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>934</v>
+      <c r="A1" s="26" t="s">
+        <v>965</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>966</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>967</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>968</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>969</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>970</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>971</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>935</v>
+        <v>972</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>936</v>
+        <v>973</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="D2" s="16" t="n">
+      <c r="D2" s="15" t="n">
         <v>0.9</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0.845</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>937</v>
+        <v>974</v>
       </c>
       <c r="G2" s="1" t="n">
         <f aca="false">C2*D2</f>
         <v>88.2</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>938</v>
+        <v>975</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>939</v>
+        <v>976</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>99.5</v>
       </c>
-      <c r="D3" s="16" t="n">
+      <c r="D3" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>0.321</v>
       </c>
-      <c r="F3" s="18" t="n">
+      <c r="F3" s="28" t="n">
         <v>4887</v>
       </c>
       <c r="G3" s="1" t="n">
@@ -75610,22 +76953,22 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>940</v>
+        <v>977</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>941</v>
+        <v>978</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="D4" s="16" t="n">
+      <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1.12</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>937</v>
+      <c r="F4" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G4" s="1" t="n">
         <f aca="false">C4*D4</f>
@@ -75634,22 +76977,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>942</v>
+        <v>979</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>943</v>
+        <v>980</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D5" s="16" t="n">
+      <c r="D5" s="15" t="n">
         <v>0.9651</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0.208</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>937</v>
+      <c r="F5" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G5" s="7" t="n">
         <f aca="false">C5*D5</f>
@@ -75659,22 +77002,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>944</v>
+        <v>981</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>945</v>
+        <v>982</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D6" s="16" t="n">
+      <c r="D6" s="15" t="n">
         <v>0.933</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.2778</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>937</v>
+      <c r="F6" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G6" s="1" t="n">
         <f aca="false">C6*D6</f>
@@ -75685,22 +77028,22 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>946</v>
+        <v>983</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>947</v>
+        <v>984</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D7" s="16" t="n">
+      <c r="D7" s="15" t="n">
         <v>0.967</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.221</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>937</v>
+      <c r="F7" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G7" s="1" t="n">
         <f aca="false">C7*D7</f>
@@ -75711,21 +77054,21 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>948</v>
+        <v>985</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>949</v>
+        <v>986</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="D8" s="16" t="n">
+      <c r="D8" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>0.233</v>
       </c>
-      <c r="F8" s="18" t="n">
+      <c r="F8" s="28" t="n">
         <v>7078.56</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -75737,22 +77080,22 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>950</v>
+        <v>987</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>951</v>
+        <v>988</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>982</v>
       </c>
-      <c r="D9" s="16" t="n">
+      <c r="D9" s="15" t="n">
         <v>0.957</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>5.689</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>937</v>
+      <c r="F9" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G9" s="7" t="n">
         <f aca="false">C9*D9</f>
@@ -75763,22 +77106,22 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>952</v>
+        <v>989</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>953</v>
+        <v>990</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D10" s="16" t="n">
+      <c r="D10" s="15" t="n">
         <v>0.944376239493814</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>3.538</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>937</v>
+      <c r="F10" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G10" s="7" t="n">
         <f aca="false">C10*D10</f>
@@ -75789,22 +77132,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>954</v>
+        <v>991</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>955</v>
+        <v>992</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="D11" s="16" t="n">
+      <c r="D11" s="15" t="n">
         <v>0.959</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>2.829</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>937</v>
+      <c r="F11" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G11" s="1" t="n">
         <f aca="false">C11*D11</f>
@@ -75813,22 +77156,22 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>956</v>
+        <v>993</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>941</v>
+        <v>978</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1060</v>
       </c>
-      <c r="D12" s="16" t="n">
+      <c r="D12" s="15" t="n">
         <v>0.974</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>7.436</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>937</v>
+      <c r="F12" s="15" t="s">
+        <v>974</v>
       </c>
       <c r="G12" s="7" t="n">
         <f aca="false">C12*D12</f>
@@ -75838,21 +77181,21 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>957</v>
+        <v>994</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>958</v>
+        <v>995</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1400</v>
       </c>
-      <c r="D13" s="16" t="n">
+      <c r="D13" s="15" t="n">
         <v>0.96</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="F13" s="19" t="n">
+      <c r="F13" s="29" t="n">
         <v>5000</v>
       </c>
       <c r="G13" s="1" t="n">
@@ -75863,7 +77206,7 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="16"/>
+      <c r="D14" s="15"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
@@ -75873,7 +77216,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="1" t="s">
-        <v>959</v>
+        <v>996</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">MEDIAN(E2:E5)</f>
@@ -75884,7 +77227,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="1" t="s">
-        <v>960</v>
+        <v>997</v>
       </c>
       <c r="G17" s="1" t="n">
         <f aca="false">MEDIAN(E9:E12)</f>

</xml_diff>

<commit_message>
Flexible production added (it can be maxed out now)
</commit_message>
<xml_diff>
--- a/Buildings/Residential/Required_energy_2014.xlsx
+++ b/Buildings/Residential/Required_energy_2014.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10201" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10204" uniqueCount="996">
   <si>
     <t xml:space="preserve">Code_BuildingVariant</t>
   </si>
@@ -2813,12 +2813,6 @@
     <t xml:space="preserve">m³</t>
   </si>
   <si>
-    <t xml:space="preserve">HP replaceable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NG + H2 boiler</t>
-  </si>
-  <si>
     <t xml:space="preserve">Heating hours per day</t>
   </si>
   <si>
@@ -2885,49 +2879,49 @@
     <t xml:space="preserve">Apartments</t>
   </si>
   <si>
-    <t xml:space="preserve">Hydrogen</t>
+    <t xml:space="preserve">% buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas demand after criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% apartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twh/yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kgH2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tot apartments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twh/yr NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MtonCO2/yr</t>
   </si>
   <si>
     <t xml:space="preserve">HP</t>
   </si>
   <si>
-    <t xml:space="preserve">H2 boiler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas demand after criteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% apartments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twh/yr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kgH2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tot apartments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Twh NG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mton CO2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mton H2</t>
   </si>
   <si>
     <t xml:space="preserve">H2</t>
   </si>
   <si>
-    <t xml:space="preserve">601 Twh is in the right order of magnitude as can be seen here : https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/natural-gas/021623-german-gas-consumption-remains-in-critical-range-in-week-6-regulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this article it is said that German consumption between 2018-21 was of 1,938 Twh/d for Households and small commercial businesses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This comes to 707.37 Twh/yr</t>
+    <t xml:space="preserve">Tot buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After criteria</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -3045,7 +3039,7 @@
     <numFmt numFmtId="172" formatCode="0.000E+00"/>
     <numFmt numFmtId="173" formatCode="0.00\ %"/>
     <numFmt numFmtId="174" formatCode="#,##0"/>
-    <numFmt numFmtId="175" formatCode="0.00000"/>
+    <numFmt numFmtId="175" formatCode="0.00\ %"/>
     <numFmt numFmtId="176" formatCode="[$£-809]#,##0.00;[RED]\-[$£-809]#,##0.00"/>
     <numFmt numFmtId="177" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
@@ -3276,7 +3270,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3353,6 +3347,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3361,7 +3359,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3655,11 +3653,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="24406194"/>
-        <c:axId val="58349270"/>
+        <c:axId val="73964855"/>
+        <c:axId val="16029879"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="24406194"/>
+        <c:axId val="73964855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3691,12 +3689,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58349270"/>
+        <c:crossAx val="16029879"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="58349270"/>
+        <c:axId val="16029879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3737,7 +3735,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24406194"/>
+        <c:crossAx val="73964855"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3775,9 +3773,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>288000</xdr:colOff>
+      <xdr:colOff>287280</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>73080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3786,7 +3784,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7758360" y="1549440"/>
-        <a:ext cx="5761080" cy="3238560"/>
+        <a:ext cx="5760360" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68484,11 +68482,11 @@
   <dimension ref="A1:BN91"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="2" topLeftCell="AZ16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="AR20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="topRight" activeCell="AZ1" activeCellId="0" sqref="AZ1"/>
-      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
-      <selection pane="bottomRight" activeCell="BI63" activeCellId="0" sqref="BI63"/>
+      <selection pane="topRight" activeCell="AR1" activeCellId="0" sqref="AR1"/>
+      <selection pane="bottomLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="BE58" activeCellId="0" sqref="BE58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -68940,9 +68938,7 @@
       <c r="AT4" s="1" t="s">
         <v>925</v>
       </c>
-      <c r="AY4" s="5" t="s">
-        <v>926</v>
-      </c>
+      <c r="AY4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
@@ -69031,21 +69027,19 @@
       <c r="AH5" s="2"/>
       <c r="AI5" s="2"/>
       <c r="AJ5" s="2"/>
-      <c r="AY5" s="6" t="s">
-        <v>927</v>
-      </c>
+      <c r="AY5" s="6"/>
       <c r="BE5" s="1"/>
       <c r="BF5" s="1"/>
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
       <c r="BI5" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="BJ5" s="1" t="n">
         <v>4.5</v>
       </c>
       <c r="BK5" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -69177,7 +69171,7 @@
       <c r="BG6" s="1"/>
       <c r="BH6" s="1"/>
       <c r="BI6" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="BJ6" s="1" t="n">
         <v>0.3</v>
@@ -69186,7 +69180,7 @@
         <v>925</v>
       </c>
       <c r="BL6" s="2" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -69303,7 +69297,7 @@
       <c r="AQ7" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR7" s="9" t="n">
+      <c r="AR7" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS7" s="1" t="n">
@@ -69318,7 +69312,7 @@
         <v>2.24806201550388</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="AW7" s="1" t="n">
         <f aca="false">AJ7*M7*AS7*1000/$BJ$17</f>
@@ -69450,7 +69444,7 @@
       <c r="AQ8" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR8" s="9" t="n">
+      <c r="AR8" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS8" s="1" t="n">
@@ -69484,7 +69478,7 @@
       <c r="BG8" s="1"/>
       <c r="BH8" s="1"/>
       <c r="BI8" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="BJ8" s="1" t="n">
         <v>5</v>
@@ -69607,7 +69601,7 @@
       <c r="AQ9" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="AR9" s="9" t="n">
+      <c r="AR9" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS9" s="1" t="n">
@@ -69747,7 +69741,7 @@
       <c r="AQ10" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR10" s="9" t="n">
+      <c r="AR10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS10" s="1" t="n">
@@ -69887,7 +69881,7 @@
       <c r="AQ11" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR11" s="9" t="n">
+      <c r="AR11" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS11" s="1" t="n">
@@ -69915,13 +69909,13 @@
       <c r="BG11" s="1"/>
       <c r="BH11" s="1"/>
       <c r="BI11" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="BJ11" s="1" t="n">
         <v>2</v>
       </c>
       <c r="BK11" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -70038,7 +70032,7 @@
       <c r="AQ12" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR12" s="9" t="n">
+      <c r="AR12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS12" s="1" t="n">
@@ -70178,7 +70172,7 @@
       <c r="AQ13" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR13" s="9" t="n">
+      <c r="AR13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS13" s="1" t="n">
@@ -70206,11 +70200,11 @@
       <c r="BE13" s="1"/>
       <c r="BF13" s="1"/>
       <c r="BG13" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="BH13" s="1"/>
       <c r="BI13" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="BJ13" s="1" t="n">
         <v>2.5</v>
@@ -70330,7 +70324,7 @@
       <c r="AQ14" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR14" s="9" t="n">
+      <c r="AR14" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS14" s="1" t="n">
@@ -70355,7 +70349,7 @@
       <c r="BA14" s="12"/>
       <c r="BB14" s="12"/>
       <c r="BC14" s="13" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="BD14" s="13"/>
       <c r="BE14" s="13"/>
@@ -70366,16 +70360,16 @@
       </c>
       <c r="BH14" s="1"/>
       <c r="BI14" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="BJ14" s="1" t="n">
         <v>14.583</v>
       </c>
       <c r="BK14" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="BM14" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="BN14" s="15" t="n">
         <v>0.94</v>
@@ -70495,7 +70489,7 @@
       <c r="AQ15" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR15" s="9" t="n">
+      <c r="AR15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS15" s="1" t="n">
@@ -70522,20 +70516,20 @@
       <c r="BE15" s="1"/>
       <c r="BF15" s="1"/>
       <c r="BG15" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="BH15" s="1"/>
       <c r="BI15" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="BJ15" s="1" t="n">
         <v>33.33</v>
       </c>
       <c r="BK15" s="1" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="BM15" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="BN15" s="15" t="n">
         <v>0.83</v>
@@ -70655,7 +70649,7 @@
       <c r="AQ16" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR16" s="9" t="n">
+      <c r="AR16" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS16" s="1" t="n">
@@ -70679,14 +70673,14 @@
       </c>
       <c r="BB16" s="1"/>
       <c r="BC16" s="12" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="BD16" s="8" t="n">
         <f aca="false">(AW15+AW16)/SUM(AW7:AW16)</f>
         <v>0.0710344522929974</v>
       </c>
       <c r="BE16" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="BG16" s="16" t="n">
         <f aca="false">BD16*SUM(AW7:AW16)/1000</f>
@@ -70813,7 +70807,7 @@
       <c r="AQ17" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR17" s="9" t="n">
+      <c r="AR17" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS17" s="1" t="n">
@@ -70834,7 +70828,7 @@
       <c r="BB17" s="1"/>
       <c r="BC17" s="1"/>
       <c r="BI17" s="1" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="BJ17" s="1" t="n">
         <v>4.987</v>
@@ -70963,7 +70957,7 @@
       <c r="AQ18" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR18" s="9" t="n">
+      <c r="AR18" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS18" s="17"/>
@@ -70984,12 +70978,14 @@
         <v>912</v>
       </c>
       <c r="BD18" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BE18" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="BF18" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="BE18" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="BF18" s="1"/>
       <c r="BG18" s="1"/>
       <c r="BH18" s="1"/>
       <c r="BI18" s="1"/>
@@ -71110,7 +71106,7 @@
       <c r="AQ19" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR19" s="9" t="n">
+      <c r="AR19" s="1" t="n">
         <v>1</v>
       </c>
       <c r="AS19" s="17"/>
@@ -71135,11 +71131,14 @@
         <f aca="false">SUM(AZ7:AZ14)</f>
         <v>9730000</v>
       </c>
-      <c r="BE19" s="1" t="n">
-        <f aca="false">BA15+BA16</f>
-        <v>184837.734806833</v>
-      </c>
-      <c r="BF19" s="18"/>
+      <c r="BE19" s="19" t="n">
+        <f aca="false">BF19/(SUM(AS7:AS16)*1000)</f>
+        <v>0.181201550387597</v>
+      </c>
+      <c r="BF19" s="18" t="n">
+        <f aca="false">(AS15+AS16)*1000</f>
+        <v>1870000</v>
+      </c>
       <c r="BG19" s="18"/>
       <c r="BH19" s="18"/>
       <c r="BI19" s="18"/>
@@ -71187,7 +71186,7 @@
         <v>0</v>
       </c>
       <c r="AQ20" s="9"/>
-      <c r="AR20" s="9"/>
+      <c r="AR20" s="1"/>
       <c r="AT20" s="10"/>
       <c r="AW20" s="1" t="n">
         <f aca="false">AJ20*M20*AS20*1000/$BJ$17</f>
@@ -71312,7 +71311,7 @@
       <c r="AQ21" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR21" s="9" t="n">
+      <c r="AR21" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS21" s="1" t="n">
@@ -71327,7 +71326,7 @@
         <v>2</v>
       </c>
       <c r="AV21" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="AW21" s="1" t="n">
         <f aca="false">AJ21*M21*AS21*1000/$BJ$17</f>
@@ -71463,7 +71462,7 @@
       <c r="AQ22" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR22" s="9" t="n">
+      <c r="AR22" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS22" s="1" t="n">
@@ -71611,7 +71610,7 @@
       <c r="AQ23" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR23" s="9" t="n">
+      <c r="AR23" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS23" s="1" t="n">
@@ -71755,7 +71754,7 @@
       <c r="AQ24" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR24" s="9" t="n">
+      <c r="AR24" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS24" s="1" t="n">
@@ -71895,7 +71894,7 @@
       <c r="AQ25" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR25" s="9" t="n">
+      <c r="AR25" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS25" s="1" t="n">
@@ -71919,7 +71918,7 @@
       </c>
       <c r="BB25" s="1"/>
       <c r="BG25" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -72038,7 +72037,7 @@
       <c r="AQ26" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR26" s="9" t="n">
+      <c r="AR26" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS26" s="1" t="n">
@@ -72062,7 +72061,7 @@
       </c>
       <c r="BB26" s="1"/>
       <c r="BC26" s="13" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="BD26" s="13"/>
       <c r="BE26" s="13"/>
@@ -72187,7 +72186,7 @@
       <c r="AQ27" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR27" s="9" t="n">
+      <c r="AR27" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS27" s="1" t="n">
@@ -72211,7 +72210,7 @@
       </c>
       <c r="BB27" s="1"/>
       <c r="BG27" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -72330,7 +72329,7 @@
       <c r="AQ28" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR28" s="9" t="n">
+      <c r="AR28" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS28" s="1" t="n">
@@ -72354,14 +72353,14 @@
       </c>
       <c r="BB28" s="1"/>
       <c r="BC28" s="12" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="BD28" s="8" t="n">
         <f aca="false">SUM(AY24:AY29)/SUM(AY21:AY29)</f>
         <v>0.529397071017861</v>
       </c>
       <c r="BE28" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="BG28" s="16" t="n">
         <f aca="false">BD28*SUM(AW21:AW29)/1000</f>
@@ -72484,7 +72483,7 @@
       <c r="AQ29" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR29" s="9" t="n">
+      <c r="AR29" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS29" s="1" t="n">
@@ -72628,7 +72627,7 @@
       <c r="AQ30" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR30" s="9" t="n">
+      <c r="AR30" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS30" s="17"/>
@@ -72653,12 +72652,14 @@
         <v>912</v>
       </c>
       <c r="BD30" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BE30" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="BF30" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="BE30" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="BF30" s="1"/>
       <c r="BG30" s="1"/>
       <c r="BH30" s="1"/>
       <c r="BI30" s="1"/>
@@ -72783,7 +72784,7 @@
       <c r="AQ31" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AR31" s="9" t="n">
+      <c r="AR31" s="1" t="n">
         <v>2</v>
       </c>
       <c r="AS31" s="17"/>
@@ -72812,11 +72813,14 @@
         <f aca="false">SUM(AZ21:AZ23)</f>
         <v>1630000</v>
       </c>
-      <c r="BE31" s="1" t="n">
-        <f aca="false">SUM(BA24:BA29)</f>
-        <v>294066.739345721</v>
-      </c>
-      <c r="BF31" s="1"/>
+      <c r="BE31" s="19" t="n">
+        <f aca="false">BF31/(SUM(AS21:AS29)*1000)</f>
+        <v>0.650963597430407</v>
+      </c>
+      <c r="BF31" s="1" t="n">
+        <f aca="false">SUM(AS24:AS29)*1000</f>
+        <v>3040000</v>
+      </c>
       <c r="BG31" s="1"/>
       <c r="BH31" s="1"/>
       <c r="BI31" s="1"/>
@@ -72990,7 +72994,7 @@
       <c r="AR33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS33" s="19" t="n">
+      <c r="AS33" s="20" t="n">
         <v>54</v>
       </c>
       <c r="AT33" s="10" t="n">
@@ -73002,7 +73006,7 @@
         <v>25.3203176704169</v>
       </c>
       <c r="AV33" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="AW33" s="1" t="n">
         <f aca="false">AJ33*M33*AS33*1000/$BJ$17</f>
@@ -73141,7 +73145,7 @@
       <c r="AR34" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS34" s="19" t="n">
+      <c r="AS34" s="20" t="n">
         <v>442</v>
       </c>
       <c r="AT34" s="10" t="n">
@@ -73285,7 +73289,7 @@
       <c r="AR35" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS35" s="19" t="n">
+      <c r="AS35" s="20" t="n">
         <v>388</v>
       </c>
       <c r="AT35" s="10" t="n">
@@ -73429,7 +73433,7 @@
       <c r="AR36" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS36" s="19" t="n">
+      <c r="AS36" s="20" t="n">
         <f aca="false">356/2</f>
         <v>178</v>
       </c>
@@ -73571,7 +73575,7 @@
       <c r="AR37" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS37" s="19" t="n">
+      <c r="AS37" s="20" t="n">
         <f aca="false">586/2</f>
         <v>293</v>
       </c>
@@ -73713,7 +73717,7 @@
       <c r="AR38" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS38" s="19" t="n">
+      <c r="AS38" s="20" t="n">
         <v>412</v>
       </c>
       <c r="AT38" s="10" t="n">
@@ -73854,7 +73858,7 @@
       <c r="AR39" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS39" s="19" t="n">
+      <c r="AS39" s="20" t="n">
         <v>146</v>
       </c>
       <c r="AT39" s="10" t="n">
@@ -73995,7 +73999,7 @@
       <c r="AR40" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS40" s="19" t="n">
+      <c r="AS40" s="20" t="n">
         <v>309</v>
       </c>
       <c r="AT40" s="10" t="n">
@@ -74136,7 +74140,7 @@
       <c r="AR41" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS41" s="19" t="n">
+      <c r="AS41" s="20" t="n">
         <v>244</v>
       </c>
       <c r="AT41" s="10" t="n">
@@ -74158,7 +74162,7 @@
       </c>
       <c r="BB41" s="1"/>
       <c r="BG41" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -74280,7 +74284,7 @@
       <c r="AR42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="AS42" s="19" t="n">
+      <c r="AS42" s="20" t="n">
         <v>85</v>
       </c>
       <c r="AT42" s="10" t="n">
@@ -74302,7 +74306,7 @@
       </c>
       <c r="BB42" s="1"/>
       <c r="BC42" s="13" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="BD42" s="13"/>
       <c r="BE42" s="13"/>
@@ -74434,7 +74438,7 @@
       <c r="AR43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS43" s="19" t="n">
+      <c r="AS43" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AT43" s="10" t="n">
@@ -74452,7 +74456,7 @@
       </c>
       <c r="BB43" s="1"/>
       <c r="BG43" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -74578,7 +74582,7 @@
       <c r="AR44" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS44" s="19" t="n">
+      <c r="AS44" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AT44" s="10" t="n">
@@ -74596,14 +74600,14 @@
       </c>
       <c r="BB44" s="1"/>
       <c r="BC44" s="12" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="BD44" s="8" t="n">
         <f aca="false">(AY33+SUM(AY36:AY42)+AY46)/SUM(AY33:AY46)</f>
         <v>0.771542772743223</v>
       </c>
       <c r="BE44" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="BG44" s="16" t="n">
         <f aca="false">BD44*SUM(AW33:AW46)/1000</f>
@@ -74729,7 +74733,7 @@
       <c r="AR45" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS45" s="19" t="n">
+      <c r="AS45" s="20" t="n">
         <f aca="false">356/2</f>
         <v>178</v>
       </c>
@@ -74874,7 +74878,7 @@
       <c r="AR46" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="AS46" s="19" t="n">
+      <c r="AS46" s="20" t="n">
         <f aca="false">586/2</f>
         <v>293</v>
       </c>
@@ -74899,12 +74903,14 @@
         <v>912</v>
       </c>
       <c r="BD46" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BE46" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="BF46" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="BE46" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="BF46" s="1"/>
       <c r="BG46" s="1"/>
       <c r="BH46" s="1"/>
       <c r="BI46" s="1"/>
@@ -74926,11 +74932,14 @@
         <f aca="false">AZ33+AZ35+AZ45</f>
         <v>3894000</v>
       </c>
-      <c r="BE47" s="1" t="n">
-        <f aca="false">SUM(BA48:BA57)</f>
-        <v>1138724.52400189</v>
-      </c>
-      <c r="BF47" s="1"/>
+      <c r="BE47" s="19" t="n">
+        <f aca="false">BF47/(SUM(AS33:AS46)*1000)</f>
+        <v>0.794837855724686</v>
+      </c>
+      <c r="BF47" s="1" t="n">
+        <f aca="false">(AS34+SUM(AS36:AS42)+AS46)*1000</f>
+        <v>2402000</v>
+      </c>
       <c r="BG47" s="1"/>
       <c r="BH47" s="1"/>
       <c r="BI47" s="1"/>
@@ -75054,7 +75063,7 @@
       <c r="AR48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS48" s="19" t="n">
+      <c r="AS48" s="20" t="n">
         <v>0.6</v>
       </c>
       <c r="AT48" s="10" t="n">
@@ -75066,7 +75075,7 @@
         <v>124.193195336664</v>
       </c>
       <c r="AV48" s="2" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="AW48" s="1" t="n">
         <f aca="false">AJ48*M48*AS48*1000/$BJ$17</f>
@@ -75201,7 +75210,7 @@
       <c r="AR49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS49" s="19" t="n">
+      <c r="AS49" s="20" t="n">
         <v>28.7</v>
       </c>
       <c r="AT49" s="10" t="n">
@@ -75349,7 +75358,7 @@
       <c r="AR50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="AS50" s="19" t="n">
+      <c r="AS50" s="20" t="n">
         <v>7.4</v>
       </c>
       <c r="AT50" s="10" t="n">
@@ -75489,7 +75498,7 @@
       <c r="AR51" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="AS51" s="19" t="n">
+      <c r="AS51" s="20" t="n">
         <v>17.3</v>
       </c>
       <c r="AT51" s="10" t="n">
@@ -75629,7 +75638,7 @@
       <c r="AR52" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="AS52" s="19" t="n">
+      <c r="AS52" s="20" t="n">
         <v>34</v>
       </c>
       <c r="AT52" s="10" t="n">
@@ -75650,7 +75659,7 @@
       </c>
       <c r="BB52" s="1"/>
       <c r="BG52" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -75772,7 +75781,7 @@
       <c r="AR53" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="AS53" s="19" t="n">
+      <c r="AS53" s="20" t="n">
         <v>50.1</v>
       </c>
       <c r="AT53" s="10" t="n">
@@ -75793,7 +75802,7 @@
       </c>
       <c r="BB53" s="1"/>
       <c r="BC53" s="13" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="BD53" s="13"/>
       <c r="BE53" s="13"/>
@@ -75921,7 +75930,7 @@
       <c r="AR54" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="AS54" s="19" t="n">
+      <c r="AS54" s="20" t="n">
         <v>15</v>
       </c>
       <c r="AT54" s="10" t="n">
@@ -75942,7 +75951,7 @@
       </c>
       <c r="BB54" s="1"/>
       <c r="BG54" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -76064,7 +76073,7 @@
       <c r="AR55" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS55" s="19" t="n">
+      <c r="AS55" s="20" t="n">
         <v>28.7</v>
       </c>
       <c r="AT55" s="10" t="n">
@@ -76085,14 +76094,14 @@
       </c>
       <c r="BB55" s="1"/>
       <c r="BC55" s="12" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="BD55" s="8" t="n">
         <f aca="false">(AY48+SUM(AY50:AY57))/SUM(AY48:AY58)</f>
         <v>0.538528362477375</v>
       </c>
       <c r="BE55" s="1" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="BG55" s="16" t="n">
         <f aca="false">BD55*SUM(AW48:AW58)/1000</f>
@@ -76218,7 +76227,7 @@
       <c r="AR56" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS56" s="19" t="n">
+      <c r="AS56" s="20" t="n">
         <v>20.9</v>
       </c>
       <c r="AT56" s="10" t="n">
@@ -76358,7 +76367,7 @@
       <c r="AR57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="AS57" s="19" t="n">
+      <c r="AS57" s="20" t="n">
         <v>7.6</v>
       </c>
       <c r="AT57" s="10" t="n">
@@ -76382,12 +76391,14 @@
         <v>912</v>
       </c>
       <c r="BD57" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="BE57" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="BF57" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="BE57" s="1" t="s">
-        <v>950</v>
-      </c>
-      <c r="BF57" s="1"/>
       <c r="BG57" s="1"/>
       <c r="BH57" s="1"/>
     </row>
@@ -76510,7 +76521,7 @@
       <c r="AR58" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="AS58" s="19" t="n">
+      <c r="AS58" s="20" t="n">
         <v>210</v>
       </c>
       <c r="AT58" s="10" t="n">
@@ -76542,11 +76553,14 @@
         <f aca="false">AZ49+AZ58</f>
         <v>8830500</v>
       </c>
-      <c r="BE58" s="1" t="n">
-        <f aca="false">SUM(BA48:BA57)/1000000</f>
-        <v>1.13872452400189</v>
-      </c>
-      <c r="BF58" s="1"/>
+      <c r="BE58" s="19" t="n">
+        <f aca="false">BF58/(SUM(AS48:AS59)*1000)</f>
+        <v>0.432072329288603</v>
+      </c>
+      <c r="BF58" s="1" t="n">
+        <f aca="false">(AS48+SUM(AS50:AS57))*1000</f>
+        <v>181600</v>
+      </c>
       <c r="BG58" s="1"/>
       <c r="BH58" s="1"/>
       <c r="BI58" s="1"/>
@@ -76670,7 +76684,7 @@
       <c r="AR59" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="AS59" s="19"/>
+      <c r="AS59" s="20"/>
       <c r="AT59" s="10" t="n">
         <f aca="false">$BJ$6*AQ59</f>
         <v>19.2</v>
@@ -76687,42 +76701,35 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="BD60" s="1" t="s">
-        <v>951</v>
-      </c>
-      <c r="BE60" s="1" t="s">
-        <v>952</v>
-      </c>
+      <c r="BE60" s="1"/>
       <c r="BG60" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="BD61" s="1" t="s">
-        <v>954</v>
-      </c>
-      <c r="BE61" s="20" t="s">
-        <v>950</v>
-      </c>
+        <v>951</v>
+      </c>
+      <c r="BE61" s="21"/>
       <c r="BG61" s="1" t="n">
         <f aca="false">(BG16+BG28+BG44+BG55)/1000000</f>
         <v>118.953912614449</v>
       </c>
       <c r="BH61" s="1" t="s">
-        <v>955</v>
-      </c>
-      <c r="BI61" s="0" t="n">
+        <v>952</v>
+      </c>
+      <c r="BI61" s="1" t="n">
         <f aca="false">BG61*1000000000/BJ15/BN15</f>
         <v>4299969007.0615</v>
       </c>
-      <c r="BJ61" s="0" t="s">
-        <v>956</v>
+      <c r="BJ61" s="1" t="s">
+        <v>953</v>
       </c>
       <c r="BK61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AR62" s="1" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="AS62" s="1" t="n">
         <f aca="false">SUMPRODUCT(AQ7:AQ59,AS7:AS59)*1000</f>
@@ -76733,79 +76740,115 @@
         <v>241.190212671658</v>
       </c>
       <c r="AX62" s="1" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="AY62" s="11" t="n">
         <f aca="false">SUM(AY7:AY59)/1000000</f>
         <v>41.3478386943115</v>
       </c>
       <c r="AZ62" s="1" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="BA62" s="1"/>
       <c r="BB62" s="1"/>
+      <c r="BC62" s="1" t="s">
+        <v>957</v>
+      </c>
       <c r="BD62" s="15" t="n">
         <f aca="false">SUM(BD19:BD58)/AS62</f>
         <v>0.298710647632816</v>
       </c>
-      <c r="BE62" s="21" t="n">
-        <f aca="false">(BE58+BE47+BE31+BE19)/1000000</f>
-        <v>1.61763013687897</v>
-      </c>
-      <c r="BF62" s="1" t="s">
-        <v>960</v>
-      </c>
-      <c r="BI62" s="0" t="n">
+      <c r="BE62" s="22"/>
+      <c r="BF62" s="1"/>
+      <c r="BI62" s="7" t="n">
         <f aca="false">BI61/1000000000</f>
         <v>4.2999690070615</v>
       </c>
-      <c r="BJ62" s="0" t="s">
-        <v>960</v>
+      <c r="BJ62" s="1" t="s">
+        <v>958</v>
       </c>
       <c r="BK62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BC63" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="BD63" s="15" t="n">
+        <f aca="false">1-BD62</f>
+        <v>0.701289352367184</v>
+      </c>
+    </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AY64" s="22" t="s">
+      <c r="AR64" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="AS64" s="1" t="n">
+        <f aca="false">SUM(AS7:AS59)*1000</f>
+        <v>18432300</v>
+      </c>
+      <c r="AY64" s="23" t="s">
         <v>912</v>
       </c>
-      <c r="AZ64" s="22"/>
+      <c r="AZ64" s="23"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AY65" s="23" t="s">
-        <v>951</v>
-      </c>
-      <c r="AZ65" s="23" t="s">
+      <c r="AY65" s="24" t="s">
+        <v>957</v>
+      </c>
+      <c r="AZ65" s="24" t="s">
+        <v>959</v>
+      </c>
+      <c r="BD65" s="1" t="s">
         <v>961</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AY66" s="24" t="n">
+      <c r="AY66" s="25" t="n">
         <f aca="false">(BC19+BC31+BC47+BC58)/1000000</f>
         <v>18.6538644760328</v>
       </c>
-      <c r="AZ66" s="24" t="n">
+      <c r="AZ66" s="25" t="n">
         <f aca="false">AY62-AY66</f>
         <v>22.6939742182788</v>
       </c>
+      <c r="BC66" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="BD66" s="15" t="n">
+        <f aca="false">1-BD67</f>
+        <v>0.593452797534762</v>
+      </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="BC67" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="BD67" s="15" t="n">
+        <f aca="false">(BF58+BF47+BF31+BF19)/AS64</f>
+        <v>0.406547202465238</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="AX68" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="AY68" s="11" t="n">
+        <f aca="false">(SUM(AY7:AY14)+AY21+AY22+AY23+AY33+AY35+AY45+AY49+AY58)/1000000</f>
+        <v>20.4790483107512</v>
+      </c>
+      <c r="AZ68" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AW69" s="25" t="s">
-        <v>962</v>
+      <c r="AW69" s="26"/>
+      <c r="AY69" s="15" t="n">
+        <f aca="false">AY68/AY62</f>
+        <v>0.495287032102325</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AW70" s="1" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AW71" s="1" t="s">
-        <v>964</v>
-      </c>
-    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -76846,9 +76889,6 @@
       <formula>$AT7&lt;$AN7</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="AW69" r:id="rId1" display="601 Twh is in the right order of magnitude as can be seen here : https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/natural-gas/021623-german-gas-consumption-remains-in-critical-range-in-week-6-regulator"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -76878,34 +76918,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
+        <v>963</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>964</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>965</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>966</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="E1" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="F1" s="27" t="s">
         <v>968</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="G1" s="27" t="s">
         <v>969</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>970</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98</v>
@@ -76917,20 +76957,20 @@
         <v>0.845</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G2" s="1" t="n">
         <f aca="false">C2*D2</f>
         <v>88.2</v>
       </c>
-      <c r="J2" s="27"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>99.5</v>
@@ -76941,7 +76981,7 @@
       <c r="E3" s="1" t="n">
         <v>0.321</v>
       </c>
-      <c r="F3" s="28" t="n">
+      <c r="F3" s="29" t="n">
         <v>4887</v>
       </c>
       <c r="G3" s="1" t="n">
@@ -76953,10 +76993,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>92</v>
@@ -76968,7 +77008,7 @@
         <v>1.12</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G4" s="1" t="n">
         <f aca="false">C4*D4</f>
@@ -76977,10 +77017,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>100</v>
@@ -76992,7 +77032,7 @@
         <v>0.208</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G5" s="7" t="n">
         <f aca="false">C5*D5</f>
@@ -77002,10 +77042,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>100</v>
@@ -77017,7 +77057,7 @@
         <v>0.2778</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G6" s="1" t="n">
         <f aca="false">C6*D6</f>
@@ -77028,10 +77068,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>100</v>
@@ -77043,7 +77083,7 @@
         <v>0.221</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G7" s="1" t="n">
         <f aca="false">C7*D7</f>
@@ -77054,10 +77094,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>95</v>
@@ -77068,7 +77108,7 @@
       <c r="E8" s="1" t="n">
         <v>0.233</v>
       </c>
-      <c r="F8" s="28" t="n">
+      <c r="F8" s="29" t="n">
         <v>7078.56</v>
       </c>
       <c r="G8" s="1" t="n">
@@ -77080,10 +77120,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>982</v>
@@ -77095,7 +77135,7 @@
         <v>5.689</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G9" s="7" t="n">
         <f aca="false">C9*D9</f>
@@ -77106,10 +77146,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>1000</v>
@@ -77121,7 +77161,7 @@
         <v>3.538</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G10" s="7" t="n">
         <f aca="false">C10*D10</f>
@@ -77132,10 +77172,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>1000</v>
@@ -77147,7 +77187,7 @@
         <v>2.829</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G11" s="1" t="n">
         <f aca="false">C11*D11</f>
@@ -77156,10 +77196,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>1060</v>
@@ -77171,7 +77211,7 @@
         <v>7.436</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G12" s="7" t="n">
         <f aca="false">C12*D12</f>
@@ -77181,10 +77221,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>1400</v>
@@ -77195,7 +77235,7 @@
       <c r="E13" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="F13" s="29" t="n">
+      <c r="F13" s="30" t="n">
         <v>5000</v>
       </c>
       <c r="G13" s="1" t="n">
@@ -77216,7 +77256,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="1" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">MEDIAN(E2:E5)</f>
@@ -77227,7 +77267,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="1" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="G17" s="1" t="n">
         <f aca="false">MEDIAN(E9:E12)</f>

</xml_diff>